<commit_message>
Ported Delete Member From Mailchimp Functionality over to v2
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/mailchimp-mailshot-sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{823B2938-BACC-0548-889C-F5A18D176212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E08810B0-5AD5-394C-92B1-612CEFCC4190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>Zendesk Field Types</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Checkbox</t>
   </si>
   <si>
-    <t>TRUE|number|Please ensure the field's 'tag' value is numeric in Zendesk|||</t>
-  </si>
-  <si>
     <t>Zenchimp Field Name</t>
   </si>
   <si>
@@ -261,6 +258,24 @@
   </si>
   <si>
     <t>LOGO</t>
+  </si>
+  <si>
+    <t>FALSE||You cannot sync from a checkbox to an Address Field|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the Zendesk field's 'tag' matches one of the Mailchimp Options, and if it's a required field in Mailchimp you need a second option is set to blank (i.e. empty text field) for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>TRUE|number|Please ensure the field's 'tag' value is numeric in Zendesk and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the field's 'tag' in Zendesk is a valid phone number and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the field's 'tag' in Zendesk is a valid website URL and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the field's 'tag' in Zendesk is a valid image URL and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
   </si>
 </sst>
 </file>
@@ -607,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -690,6 +705,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1112,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA687FE-D53D-0F4D-87AF-8ACBE173826C}">
   <dimension ref="A1:P999"/>
   <sheetViews>
-    <sheetView topLeftCell="L2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1161,7 +1179,7 @@
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1176,35 +1194,35 @@
     </row>
     <row r="3" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="21">
         <v>1</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="23">
         <v>3</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="2">
         <v>4</v>
@@ -1216,18 +1234,18 @@
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>1</v>
@@ -1251,7 +1269,7 @@
         <f t="shared" ref="J4:J16" si="2">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(3-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="K4" s="8" t="str">
+      <c r="K4" s="43" t="str">
         <f t="shared" ref="K4:K7" si="3">IF(H4="", "", IF( J4="", IF( H4="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H4="TRUE", CONCATENATE("Valid, but: ", J4), CONCATENATE("INVALID - FIELD EXCLUDED: ", J4))))</f>
         <v/>
       </c>
@@ -1274,22 +1292,22 @@
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="8" t="str">
         <f t="array" ref="G5">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C5,Hidden!$A$2:$A$9,0), MATCH($E5,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C5,Hidden!$A$2:$A$9,0), MATCH($E5,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
@@ -1307,7 +1325,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K5" s="8" t="str">
+      <c r="K5" s="43" t="str">
         <f t="shared" si="3"/>
         <v>Valid</v>
       </c>
@@ -1341,16 +1359,16 @@
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>10</v>
@@ -1372,7 +1390,7 @@
         <f t="shared" si="2"/>
         <v>Please use full URLs when entering values in Zendesk</v>
       </c>
-      <c r="K6" s="8" t="str">
+      <c r="K6" s="43" t="str">
         <f t="shared" si="3"/>
         <v>Valid, but: Please use full URLs when entering values in Zendesk</v>
       </c>
@@ -1427,7 +1445,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K7" s="8" t="str">
+      <c r="K7" s="43" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1475,7 +1493,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K8" s="8" t="str">
+      <c r="K8" s="43" t="str">
         <f>IF(H8="", "", IF( J8="", IF( H8="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H8="TRUE", CONCATENATE("Valid, but: ", J8), CONCATENATE("INVALID - FIELD EXCLUDED: ", J8))))</f>
         <v/>
       </c>
@@ -1523,7 +1541,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K9" s="8" t="str">
+      <c r="K9" s="43" t="str">
         <f t="shared" ref="K9:K16" si="9">IF(H9="", "", IF( J9="", IF( H9="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H9="TRUE", CONCATENATE("Valid, but: ", J9), CONCATENATE("INVALID - FIELD EXCLUDED: ", J9))))</f>
         <v/>
       </c>
@@ -1571,7 +1589,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K10" s="8" t="str">
+      <c r="K10" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1619,7 +1637,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="8" t="str">
+      <c r="K11" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1667,7 +1685,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="8" t="str">
+      <c r="K12" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1715,7 +1733,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="8" t="str">
+      <c r="K13" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1763,7 +1781,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="8" t="str">
+      <c r="K14" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1811,7 +1829,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="8" t="str">
+      <c r="K15" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1859,7 +1877,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="8" t="str">
+      <c r="K16" s="43" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -2932,7 +2950,7 @@
   <dimension ref="A1:P1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2994,35 +3012,35 @@
     </row>
     <row r="3" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="21">
         <v>1</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="23">
         <v>3</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="2">
         <v>4</v>
@@ -3034,24 +3052,24 @@
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>1</v>
@@ -3072,7 +3090,7 @@
         <f t="shared" ref="J4:J18" si="1">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(3-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="K4" s="8" t="str">
+      <c r="K4" s="43" t="str">
         <f t="shared" ref="K4:K18" si="2">IF(H4="", "", IF( J4="", IF( H4="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H4="TRUE", CONCATENATE("Valid, but: ", J4), CONCATENATE("INVALID - FIELD EXCLUDED: ", J4))))</f>
         <v>Valid</v>
       </c>
@@ -3098,7 +3116,7 @@
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
       <c r="D5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>1</v>
@@ -3119,7 +3137,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K5" s="8" t="str">
+      <c r="K5" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3142,16 +3160,16 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>1</v>
@@ -3173,7 +3191,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K6" s="8" t="str">
+      <c r="K6" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3196,22 +3214,22 @@
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="8" t="str">
         <f t="array" ref="G7">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
@@ -3229,7 +3247,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K7" s="8" t="str">
+      <c r="K7" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3263,16 +3281,16 @@
     </row>
     <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>1</v>
@@ -3294,7 +3312,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K8" s="8" t="str">
+      <c r="K8" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3328,16 +3346,16 @@
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>3</v>
@@ -3359,7 +3377,7 @@
         <f t="shared" si="1"/>
         <v>Unsupported Field Type Combination</v>
       </c>
-      <c r="K9" s="8" t="str">
+      <c r="K9" s="43" t="str">
         <f t="shared" si="2"/>
         <v>INVALID - FIELD EXCLUDED: Unsupported Field Type Combination</v>
       </c>
@@ -3386,16 +3404,16 @@
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>6</v>
@@ -3417,7 +3435,7 @@
         <f t="shared" si="1"/>
         <v>Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)</v>
       </c>
-      <c r="K10" s="8" t="str">
+      <c r="K10" s="43" t="str">
         <f>IF(H10="", "", IF( J10="", IF( H10="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H10="TRUE", CONCATENATE("Valid, but: ", J10), CONCATENATE("INVALID - FIELD EXCLUDED: ", J10))))</f>
         <v>INVALID - FIELD EXCLUDED: Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)</v>
       </c>
@@ -3465,7 +3483,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="8" t="str">
+      <c r="K11" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3513,7 +3531,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="8" t="str">
+      <c r="K12" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3561,7 +3579,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="8" t="str">
+      <c r="K13" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3609,7 +3627,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K14" s="8" t="str">
+      <c r="K14" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3657,7 +3675,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="8" t="str">
+      <c r="K15" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3705,7 +3723,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="8" t="str">
+      <c r="K16" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3753,7 +3771,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="8" t="str">
+      <c r="K17" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3801,7 +3819,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K18" s="8" t="str">
+      <c r="K18" s="43" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4876,8 +4894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4944,7 +4962,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -4973,7 +4991,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5008,7 +5026,7 @@
         <v>24</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5033,7 +5051,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5058,43 +5076,53 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>76</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="H7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>79</v>
+      </c>
       <c r="K7" s="26" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -5108,7 +5136,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5131,7 +5159,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improving Type Compatibility between Zendesk and Mailchimp fields
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/mailchimp-mailshot-sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E08810B0-5AD5-394C-92B1-612CEFCC4190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AEBC61-1140-864A-988F-A755CA464603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zendesk Organisation Fields" sheetId="4" r:id="rId1"/>
@@ -74,15 +74,9 @@
     <t>TRUE|text</t>
   </si>
   <si>
-    <t>TRUE|number|Please ensure the 'tag' values are all numeric in Zendesk when adding your drop down options|||</t>
-  </si>
-  <si>
     <t>FALSE||Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)|||</t>
   </si>
   <si>
-    <t>TRUE|number|Your sync will fail if you enter a non-numeric value in your zendesk field|||</t>
-  </si>
-  <si>
     <t>TRUE|text|Your sync will fail if your zendesk value does not match one of the Mailchimp options|||</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Numeric</t>
   </si>
   <si>
-    <t>TRUE|number||||</t>
-  </si>
-  <si>
     <t>Decimal</t>
   </si>
   <si>
@@ -128,9 +119,6 @@
     <t>Regular Expression</t>
   </si>
   <si>
-    <t>TRUE|number|Please ensure the regular expression only allows numeric values|||</t>
-  </si>
-  <si>
     <t>Zendesk Field Key</t>
   </si>
   <si>
@@ -266,9 +254,6 @@
     <t>TRUE|text|Please ensure the Zendesk field's 'tag' matches one of the Mailchimp Options, and if it's a required field in Mailchimp you need a second option is set to blank (i.e. empty text field) for when the checkbox is unticked|||</t>
   </si>
   <si>
-    <t>TRUE|number|Please ensure the field's 'tag' value is numeric in Zendesk and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
-  </si>
-  <si>
     <t>TRUE|text|Please ensure the field's 'tag' in Zendesk is a valid phone number and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
   </si>
   <si>
@@ -276,13 +261,28 @@
   </si>
   <si>
     <t>TRUE|text|Please ensure the field's 'tag' in Zendesk is a valid image URL and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the 'tag' values are all numeric in Zendesk when adding your drop down options|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Your sync will fail if you enter a non-numeric value in your zendesk field|||</t>
+  </si>
+  <si>
+    <t>TRUE|text||||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the field's 'tag' value is numeric in Zendesk and the field is set to 'not required' in Mailchimp for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the regular expression only allows numeric values|||</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,12 +312,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -620,57 +614,51 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -680,34 +668,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1130,32 +1118,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA687FE-D53D-0F4D-87AF-8ACBE173826C}">
   <dimension ref="A1:P999"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" style="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="11" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="107" style="11" customWidth="1"/>
-    <col min="12" max="16" width="10.7109375" style="11" customWidth="1"/>
-    <col min="17" max="26" width="10.5703125" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="11.28515625" style="11"/>
+    <col min="1" max="1" width="26.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="9" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="107" style="9" customWidth="1"/>
+    <col min="12" max="16" width="10.7109375" style="9" customWidth="1"/>
+    <col min="17" max="26" width="10.5703125" style="9" customWidth="1"/>
+    <col min="27" max="16384" width="11.28515625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="270" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="29" t="str">
+      <c r="I1" s="28" t="str">
         <f>CONCATENATE("[",CHAR(10), $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$313, $O$14, $O$15, $O$16,"]")</f>
         <v>[
   {
@@ -1174,55 +1162,55 @@
   }
 ]</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="A2" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="D3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="19">
+        <v>1</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="21">
+        <v>3</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21">
-        <v>1</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="23">
-        <v>3</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>37</v>
       </c>
       <c r="L3" s="2">
         <v>4</v>
@@ -1234,34 +1222,34 @@
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="A4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="8" t="str">
+      <c r="D4" s="4"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="6" t="str">
         <f t="array" ref="G4">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C4,Hidden!$A$2:$A$9,0), MATCH($E4,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C4,Hidden!$A$2:$A$9,0), MATCH($E4,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H4" s="8" t="str">
+      <c r="H4" s="6" t="str">
         <f t="shared" ref="H4:H16" si="0">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(1-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="I4" s="16" t="str">
+      <c r="I4" s="14" t="str">
         <f t="shared" ref="I4:I16" si="1">IF(H4="","",IF(H4="TRUE",TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(2-1)*LEN($G4)+1,LEN($G4))),"-"))</f>
         <v/>
       </c>
@@ -1269,7 +1257,7 @@
         <f t="shared" ref="J4:J16" si="2">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(3-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="K4" s="43" t="str">
+      <c r="K4" s="27" t="str">
         <f t="shared" ref="K4:K7" si="3">IF(H4="", "", IF( J4="", IF( H4="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H4="TRUE", CONCATENATE("Valid, but: ", J4), CONCATENATE("INVALID - FIELD EXCLUDED: ", J4))))</f>
         <v/>
       </c>
@@ -1291,33 +1279,33 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="8" t="str">
+      <c r="F5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="6" t="str">
         <f t="array" ref="G5">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C5,Hidden!$A$2:$A$9,0), MATCH($E5,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C5,Hidden!$A$2:$A$9,0), MATCH($E5,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
       </c>
-      <c r="H5" s="8" t="str">
+      <c r="H5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I5" s="16" t="str">
+      <c r="I5" s="14" t="str">
         <f t="shared" si="1"/>
         <v>text</v>
       </c>
@@ -1325,7 +1313,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K5" s="43" t="str">
+      <c r="K5" s="27" t="str">
         <f t="shared" si="3"/>
         <v>Valid</v>
       </c>
@@ -1358,31 +1346,31 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8" t="str">
+      <c r="F6" s="7"/>
+      <c r="G6" s="6" t="str">
         <f t="array" ref="G6">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C6,Hidden!$A$2:$A$9,0), MATCH($E6,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C6,Hidden!$A$2:$A$9,0), MATCH($E6,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|image|Please use full URLs when entering values in Zendesk|||</v>
       </c>
-      <c r="H6" s="8" t="str">
+      <c r="H6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I6" s="16" t="str">
+      <c r="I6" s="14" t="str">
         <f t="shared" si="1"/>
         <v>image</v>
       </c>
@@ -1390,7 +1378,7 @@
         <f t="shared" si="2"/>
         <v>Please use full URLs when entering values in Zendesk</v>
       </c>
-      <c r="K6" s="43" t="str">
+      <c r="K6" s="27" t="str">
         <f t="shared" si="3"/>
         <v>Valid, but: Please use full URLs when entering values in Zendesk</v>
       </c>
@@ -1423,21 +1411,21 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8" t="str">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6" t="str">
         <f t="array" ref="G7">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="H7" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I7" s="16" t="str">
+      <c r="I7" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1445,7 +1433,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K7" s="43" t="str">
+      <c r="K7" s="27" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1471,21 +1459,21 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8" t="str">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6" t="str">
         <f t="array" ref="G8">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C8,Hidden!$A$2:$A$9,0), MATCH($E8,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C8,Hidden!$A$2:$A$9,0), MATCH($E8,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H8" s="8" t="str">
+      <c r="H8" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I8" s="16" t="str">
+      <c r="I8" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1493,7 +1481,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K8" s="43" t="str">
+      <c r="K8" s="27" t="str">
         <f>IF(H8="", "", IF( J8="", IF( H8="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H8="TRUE", CONCATENATE("Valid, but: ", J8), CONCATENATE("INVALID - FIELD EXCLUDED: ", J8))))</f>
         <v/>
       </c>
@@ -1519,21 +1507,21 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8" t="str">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6" t="str">
         <f t="array" ref="G9">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C9,Hidden!$A$2:$A$9,0), MATCH($E9,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C9,Hidden!$A$2:$A$9,0), MATCH($E9,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="H9" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I9" s="16" t="str">
+      <c r="I9" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1541,7 +1529,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K9" s="43" t="str">
+      <c r="K9" s="27" t="str">
         <f t="shared" ref="K9:K16" si="9">IF(H9="", "", IF( J9="", IF( H9="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H9="TRUE", CONCATENATE("Valid, but: ", J9), CONCATENATE("INVALID - FIELD EXCLUDED: ", J9))))</f>
         <v/>
       </c>
@@ -1567,21 +1555,21 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8" t="str">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="str">
         <f t="array" ref="G10">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C10,Hidden!$A$2:$A$9,0), MATCH($E10,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C10,Hidden!$A$2:$A$9,0), MATCH($E10,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H10" s="8" t="str">
+      <c r="H10" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I10" s="16" t="str">
+      <c r="I10" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1589,7 +1577,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K10" s="43" t="str">
+      <c r="K10" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1615,21 +1603,21 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8" t="str">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6" t="str">
         <f t="array" ref="G11">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C11,Hidden!$A$2:$A$9,0), MATCH($E11,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C11,Hidden!$A$2:$A$9,0), MATCH($E11,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H11" s="8" t="str">
+      <c r="H11" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I11" s="16" t="str">
+      <c r="I11" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1637,7 +1625,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="43" t="str">
+      <c r="K11" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1663,21 +1651,21 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8" t="str">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="str">
         <f t="array" ref="G12">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C12,Hidden!$A$2:$A$9,0), MATCH($E12,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C12,Hidden!$A$2:$A$9,0), MATCH($E12,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H12" s="8" t="str">
+      <c r="H12" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I12" s="16" t="str">
+      <c r="I12" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1685,7 +1673,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="43" t="str">
+      <c r="K12" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1711,21 +1699,21 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8" t="str">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6" t="str">
         <f t="array" ref="G13">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C13,Hidden!$A$2:$A$9,0), MATCH($E13,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C13,Hidden!$A$2:$A$9,0), MATCH($E13,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="H13" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I13" s="16" t="str">
+      <c r="I13" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1733,7 +1721,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="43" t="str">
+      <c r="K13" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1759,21 +1747,21 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8" t="str">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6" t="str">
         <f t="array" ref="G14">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C14,Hidden!$A$2:$A$9,0), MATCH($E14,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C14,Hidden!$A$2:$A$9,0), MATCH($E14,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H14" s="8" t="str">
+      <c r="H14" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I14" s="16" t="str">
+      <c r="I14" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1781,7 +1769,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="43" t="str">
+      <c r="K14" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1807,21 +1795,21 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="8" t="str">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6" t="str">
         <f t="array" ref="G15">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C15,Hidden!$A$2:$A$9,0), MATCH($E15,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C15,Hidden!$A$2:$A$9,0), MATCH($E15,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H15" s="8" t="str">
+      <c r="H15" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I15" s="16" t="str">
+      <c r="I15" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1829,7 +1817,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="43" t="str">
+      <c r="K15" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1855,21 +1843,21 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8" t="str">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="6" t="str">
         <f t="array" ref="G16">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C16,Hidden!$A$2:$A$9,0), MATCH($E16,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C16,Hidden!$A$2:$A$9,0), MATCH($E16,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H16" s="8" t="str">
+      <c r="H16" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I16" s="16" t="str">
+      <c r="I16" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1877,7 +1865,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="43" t="str">
+      <c r="K16" s="27" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -2949,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2973,7 +2961,7 @@
     <row r="1" spans="1:16" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="37" t="str">
+      <c r="I1" s="36" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$14, $O$315, $O$16, $O$17, $O$18,"]")</f>
         <v>[
   {
@@ -2992,55 +2980,55 @@
   }
 ]</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
+      <c r="A2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
     </row>
     <row r="3" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="D3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="19">
+        <v>1</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="21">
+        <v>3</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21">
-        <v>1</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="23">
-        <v>3</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>37</v>
       </c>
       <c r="L3" s="2">
         <v>4</v>
@@ -3052,37 +3040,37 @@
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="8" t="str">
+      <c r="H4" s="6" t="str">
         <f t="shared" ref="H4:H18" si="0">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(1-1)*LEN($G4)+1,LEN($G4)))</f>
         <v>TRUE</v>
       </c>
-      <c r="I4" s="16" t="str">
+      <c r="I4" s="14" t="str">
         <f>IF(H4="","",IF(H4="TRUE",TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(2-1)*LEN($G4)+1,LEN($G4))),"-"))</f>
         <v>text</v>
       </c>
@@ -3090,7 +3078,7 @@
         <f t="shared" ref="J4:J18" si="1">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(3-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="K4" s="43" t="str">
+      <c r="K4" s="27" t="str">
         <f t="shared" ref="K4:K18" si="2">IF(H4="", "", IF( J4="", IF( H4="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H4="TRUE", CONCATENATE("Valid, but: ", J4), CONCATENATE("INVALID - FIELD EXCLUDED: ", J4))))</f>
         <v>Valid</v>
       </c>
@@ -3112,24 +3100,24 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8" t="str">
+      <c r="H5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I5" s="16" t="str">
+      <c r="I5" s="14" t="str">
         <f t="shared" ref="I5:I18" si="7">IF(H5="","",IF(H5="TRUE",TRIM(MID(SUBSTITUTE($G5,"|",REPT(" ",LEN($G5))),(2-1)*LEN($G5)+1,LEN($G5))),"-"))</f>
         <v>text</v>
       </c>
@@ -3137,7 +3125,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K5" s="43" t="str">
+      <c r="K5" s="27" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3159,31 +3147,31 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="A6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="8" t="str">
+      <c r="F6" s="12"/>
+      <c r="G6" s="6" t="str">
         <f t="array" ref="G6">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C6,Hidden!$A$2:$A$9,0), MATCH($E6,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C6,Hidden!$A$2:$A$9,0), MATCH($E6,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
       </c>
-      <c r="H6" s="8" t="str">
+      <c r="H6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I6" s="16" t="str">
+      <c r="I6" s="14" t="str">
         <f t="shared" si="7"/>
         <v>text</v>
       </c>
@@ -3191,7 +3179,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K6" s="43" t="str">
+      <c r="K6" s="27" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3213,33 +3201,33 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="8" t="str">
+      <c r="F7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="6" t="str">
         <f t="array" ref="G7">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="H7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I7" s="16" t="str">
+      <c r="I7" s="14" t="str">
         <f t="shared" si="7"/>
         <v>text</v>
       </c>
@@ -3247,7 +3235,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K7" s="43" t="str">
+      <c r="K7" s="27" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3280,31 +3268,31 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="A8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8" t="str">
+      <c r="F8" s="7"/>
+      <c r="G8" s="6" t="str">
         <f t="array" ref="G8">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C8,Hidden!$A$2:$A$9,0), MATCH($E8,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C8,Hidden!$A$2:$A$9,0), MATCH($E8,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
       </c>
-      <c r="H8" s="8" t="str">
+      <c r="H8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I8" s="16" t="str">
+      <c r="I8" s="14" t="str">
         <f t="shared" si="7"/>
         <v>text</v>
       </c>
@@ -3312,7 +3300,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K8" s="43" t="str">
+      <c r="K8" s="27" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3345,31 +3333,31 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="A9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8" t="str">
+      <c r="F9" s="7"/>
+      <c r="G9" s="6" t="str">
         <f t="array" ref="G9">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C9,Hidden!$A$2:$A$9,0), MATCH($E9,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C9,Hidden!$A$2:$A$9,0), MATCH($E9,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>FALSE||Unsupported Field Type Combination|||</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="H9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="I9" s="16" t="str">
+      <c r="I9" s="14" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
@@ -3377,7 +3365,7 @@
         <f t="shared" si="1"/>
         <v>Unsupported Field Type Combination</v>
       </c>
-      <c r="K9" s="43" t="str">
+      <c r="K9" s="27" t="str">
         <f t="shared" si="2"/>
         <v>INVALID - FIELD EXCLUDED: Unsupported Field Type Combination</v>
       </c>
@@ -3403,31 +3391,31 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8" t="str">
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="str">
         <f t="array" ref="G10">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C10,Hidden!$A$2:$A$9,0), MATCH($E10,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C10,Hidden!$A$2:$A$9,0), MATCH($E10,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>FALSE||Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)|||</v>
       </c>
-      <c r="H10" s="8" t="str">
+      <c r="H10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="I10" s="16" t="str">
+      <c r="I10" s="14" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
@@ -3435,7 +3423,7 @@
         <f t="shared" si="1"/>
         <v>Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)</v>
       </c>
-      <c r="K10" s="43" t="str">
+      <c r="K10" s="27" t="str">
         <f>IF(H10="", "", IF( J10="", IF( H10="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H10="TRUE", CONCATENATE("Valid, but: ", J10), CONCATENATE("INVALID - FIELD EXCLUDED: ", J10))))</f>
         <v>INVALID - FIELD EXCLUDED: Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)</v>
       </c>
@@ -3461,21 +3449,21 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8" t="str">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6" t="str">
         <f t="array" ref="G11">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C11,Hidden!$A$2:$A$9,0), MATCH($E11,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C11,Hidden!$A$2:$A$9,0), MATCH($E11,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H11" s="8" t="str">
+      <c r="H11" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I11" s="16" t="str">
+      <c r="I11" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3483,7 +3471,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="43" t="str">
+      <c r="K11" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3509,21 +3497,21 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8" t="str">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="str">
         <f t="array" ref="G12">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C12,Hidden!$A$2:$A$9,0), MATCH($E12,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C12,Hidden!$A$2:$A$9,0), MATCH($E12,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H12" s="8" t="str">
+      <c r="H12" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I12" s="16" t="str">
+      <c r="I12" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3531,7 +3519,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="43" t="str">
+      <c r="K12" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3557,21 +3545,21 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8" t="str">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6" t="str">
         <f t="array" ref="G13">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C13,Hidden!$A$2:$A$9,0), MATCH($E13,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C13,Hidden!$A$2:$A$9,0), MATCH($E13,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="H13" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I13" s="16" t="str">
+      <c r="I13" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3579,7 +3567,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="43" t="str">
+      <c r="K13" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3605,21 +3593,21 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8" t="str">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6" t="str">
         <f t="array" ref="G14">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C14,Hidden!$A$2:$A$9,0), MATCH($E14,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C14,Hidden!$A$2:$A$9,0), MATCH($E14,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H14" s="8" t="str">
+      <c r="H14" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I14" s="16" t="str">
+      <c r="I14" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3627,7 +3615,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K14" s="43" t="str">
+      <c r="K14" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3653,21 +3641,21 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="8" t="str">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6" t="str">
         <f t="array" ref="G15">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C15,Hidden!$A$2:$A$9,0), MATCH($E15,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C15,Hidden!$A$2:$A$9,0), MATCH($E15,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H15" s="8" t="str">
+      <c r="H15" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I15" s="16" t="str">
+      <c r="I15" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3675,7 +3663,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="43" t="str">
+      <c r="K15" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3701,21 +3689,21 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8" t="str">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="6" t="str">
         <f t="array" ref="G16">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C16,Hidden!$A$2:$A$9,0), MATCH($E16,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C16,Hidden!$A$2:$A$9,0), MATCH($E16,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H16" s="8" t="str">
+      <c r="H16" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I16" s="16" t="str">
+      <c r="I16" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3723,7 +3711,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="43" t="str">
+      <c r="K16" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3749,21 +3737,21 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8" t="str">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="6" t="str">
         <f t="array" ref="G17">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C17,Hidden!$A$2:$A$9,0), MATCH($E17,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C17,Hidden!$A$2:$A$9,0), MATCH($E17,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="H17" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I17" s="16" t="str">
+      <c r="I17" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3771,7 +3759,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="43" t="str">
+      <c r="K17" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3797,21 +3785,21 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8" t="str">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6" t="str">
         <f t="array" ref="G18">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C18,Hidden!$A$2:$A$9,0), MATCH($E18,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C18,Hidden!$A$2:$A$9,0), MATCH($E18,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
       </c>
-      <c r="H18" s="8" t="str">
+      <c r="H18" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I18" s="16" t="str">
+      <c r="I18" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -3819,7 +3807,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K18" s="43" t="str">
+      <c r="K18" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4895,271 +4883,271 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="28" customWidth="1"/>
-    <col min="2" max="11" width="29" style="28" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="26" customWidth="1"/>
+    <col min="2" max="11" width="29" style="26" customWidth="1"/>
     <col min="12" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="26" t="s">
-        <v>69</v>
+      <c r="G2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="26" t="s">
-        <v>70</v>
+      <c r="F3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="I4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>70</v>
+      <c r="K4" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="26" t="s">
-        <v>72</v>
+      <c r="C5" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="26" t="s">
-        <v>72</v>
+      <c r="C6" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="26" t="s">
+      <c r="C7" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>75</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="26" t="s">
-        <v>71</v>
+      <c r="C8" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="26" t="s">
-        <v>72</v>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Porting to V2 for use in user_sidebar location
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/mailchimp-mailshot-sync/extras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/ZenChimp-Zendesk-App-Mailchimp-Sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AEBC61-1140-864A-988F-A755CA464603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43844E7B-102A-E046-A063-88DE8B110122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zendesk Organisation Fields" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t>Zendesk Field Types</t>
   </si>
@@ -95,9 +95,6 @@
     <t>FALSE||A multi line text field is used for storing paragrahps of text, this will not sync to a drop down|||</t>
   </si>
   <si>
-    <t>FALSE||A multi line text field is used for storing paragrahps of text, this will not sync to an address field|||</t>
-  </si>
-  <si>
     <t>FALSE||A multi line text field is used for storing paragrahps of text, this will not sync to a Phone number field|||</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>sdfsdfsdf</t>
   </si>
   <si>
-    <t>ZenChimp Field Type</t>
-  </si>
-  <si>
     <t>User's Name</t>
   </si>
   <si>
@@ -248,9 +242,6 @@
     <t>LOGO</t>
   </si>
   <si>
-    <t>FALSE||You cannot sync from a checkbox to an Address Field|||</t>
-  </si>
-  <si>
     <t>TRUE|text|Please ensure the Zendesk field's 'tag' matches one of the Mailchimp Options, and if it's a required field in Mailchimp you need a second option is set to blank (i.e. empty text field) for when the checkbox is unticked|||</t>
   </si>
   <si>
@@ -276,13 +267,37 @@
   </si>
   <si>
     <t>TRUE|text|Please ensure the regular expression only allows numeric values|||</t>
+  </si>
+  <si>
+    <t>No of Employees</t>
+  </si>
+  <si>
+    <t>no_of_employees</t>
+  </si>
+  <si>
+    <t>EMPLOYEES</t>
+  </si>
+  <si>
+    <t>FALSE||Syncing to Address fields is not yet supported by Zenchimp, use a Text field in Mailchimp (or one per line of address for long addresses) or raise a feature request on github :)|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Numbers with more than two decimal places show as out-of-sync as mailchimp has a limit of 2 decimal places|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Make sure your Zendesk 'tag' values match the Mailchimp 'Options' for the field exactly|||</t>
+  </si>
+  <si>
+    <t>TRUE|text|Please ensure the Zendesk field's 'tag' matches one of the Mailchimp Options, and if it's a required field in Mailchimp you need a second option set to blank (i.e. empty text field) for when the checkbox is unticked|||</t>
+  </si>
+  <si>
+    <t>ZenChimp Data Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,13 +405,6 @@
       <sz val="10"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF44546A"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -614,7 +622,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -649,16 +657,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -696,6 +701,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1118,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA687FE-D53D-0F4D-87AF-8ACBE173826C}">
   <dimension ref="A1:P999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1151,7 @@
     <row r="1" spans="1:16" ht="270" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="28" t="str">
+      <c r="I1" s="27" t="str">
         <f>CONCATENATE("[",CHAR(10), $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$313, $O$14, $O$15, $O$16,"]")</f>
         <v>[
   {
@@ -1160,57 +1168,64 @@
     "type" : "image",
     "default_value" : ""
   }
+ ,{
+    "field_label" : "No of Employees",
+    "zendesk_field" : "no_of_employees",
+    "mailchimp_field" : "EMPLOYEES",
+    "type" : "text",
+    "default_value" : ""
+  }
 ]</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="A2" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="19">
         <v>1</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="21">
+      <c r="I3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="20">
         <v>3</v>
       </c>
-      <c r="K3" s="22" t="s">
-        <v>33</v>
+      <c r="K3" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="L3" s="2">
         <v>4</v>
@@ -1222,25 +1237,25 @@
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="6" t="str">
         <f t="array" ref="G4">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C4,Hidden!$A$2:$A$9,0), MATCH($E4,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C4,Hidden!$A$2:$A$9,0), MATCH($E4,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>|||||</v>
@@ -1257,7 +1272,7 @@
         <f t="shared" ref="J4:J16" si="2">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(3-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="K4" s="27" t="str">
+      <c r="K4" s="26" t="str">
         <f t="shared" ref="K4:K7" si="3">IF(H4="", "", IF( J4="", IF( H4="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H4="TRUE", CONCATENATE("Valid, but: ", J4), CONCATENATE("INVALID - FIELD EXCLUDED: ", J4))))</f>
         <v/>
       </c>
@@ -1280,22 +1295,22 @@
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5" s="6" t="str">
         <f t="array" ref="G5">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C5,Hidden!$A$2:$A$9,0), MATCH($E5,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C5,Hidden!$A$2:$A$9,0), MATCH($E5,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
@@ -1313,7 +1328,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K5" s="27" t="str">
+      <c r="K5" s="26" t="str">
         <f t="shared" si="3"/>
         <v>Valid</v>
       </c>
@@ -1347,16 +1362,16 @@
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>10</v>
@@ -1378,7 +1393,7 @@
         <f t="shared" si="2"/>
         <v>Please use full URLs when entering values in Zendesk</v>
       </c>
-      <c r="K6" s="27" t="str">
+      <c r="K6" s="26" t="str">
         <f t="shared" si="3"/>
         <v>Valid, but: Please use full URLs when entering values in Zendesk</v>
       </c>
@@ -1411,31 +1426,41 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="6" t="str">
         <f t="array" ref="G7">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
-        <v>|||||</v>
+        <v>TRUE|text||||</v>
       </c>
       <c r="H7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>TRUE</v>
       </c>
       <c r="I7" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>text</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K7" s="27" t="str">
+      <c r="K7" s="26" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Valid</v>
       </c>
       <c r="L7" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1451,7 +1476,14 @@
       </c>
       <c r="O7" s="2" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v xml:space="preserve"> ,{
+    "field_label" : "No of Employees",
+    "zendesk_field" : "no_of_employees",
+    "mailchimp_field" : "EMPLOYEES",
+    "type" : "text",
+    "default_value" : ""
+  }
+</v>
       </c>
       <c r="P7" s="2" t="str">
         <f t="shared" si="7"/>
@@ -1481,7 +1513,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K8" s="27" t="str">
+      <c r="K8" s="26" t="str">
         <f>IF(H8="", "", IF( J8="", IF( H8="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H8="TRUE", CONCATENATE("Valid, but: ", J8), CONCATENATE("INVALID - FIELD EXCLUDED: ", J8))))</f>
         <v/>
       </c>
@@ -1529,7 +1561,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K9" s="27" t="str">
+      <c r="K9" s="26" t="str">
         <f t="shared" ref="K9:K16" si="9">IF(H9="", "", IF( J9="", IF( H9="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H9="TRUE", CONCATENATE("Valid, but: ", J9), CONCATENATE("INVALID - FIELD EXCLUDED: ", J9))))</f>
         <v/>
       </c>
@@ -1577,7 +1609,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K10" s="27" t="str">
+      <c r="K10" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1625,7 +1657,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="27" t="str">
+      <c r="K11" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1673,7 +1705,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="27" t="str">
+      <c r="K12" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1721,7 +1753,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="27" t="str">
+      <c r="K13" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1769,7 +1801,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="27" t="str">
+      <c r="K14" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1817,7 +1849,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="27" t="str">
+      <c r="K15" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -1865,7 +1897,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="27" t="str">
+      <c r="K16" s="26" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -2937,8 +2969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2961,7 +2993,7 @@
     <row r="1" spans="1:16" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="36" t="str">
+      <c r="I1" s="35" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$14, $O$315, $O$16, $O$17, $O$18,"]")</f>
         <v>[
   {
@@ -2980,55 +3012,55 @@
   }
 ]</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="19">
         <v>1</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="21">
+      <c r="I3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="20">
         <v>3</v>
       </c>
-      <c r="K3" s="22" t="s">
-        <v>33</v>
+      <c r="K3" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="L3" s="2">
         <v>4</v>
@@ -3040,24 +3072,24 @@
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>1</v>
@@ -3078,7 +3110,7 @@
         <f t="shared" ref="J4:J18" si="1">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(3-1)*LEN($G4)+1,LEN($G4)))</f>
         <v/>
       </c>
-      <c r="K4" s="27" t="str">
+      <c r="K4" s="26" t="str">
         <f t="shared" ref="K4:K18" si="2">IF(H4="", "", IF( J4="", IF( H4="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H4="TRUE", CONCATENATE("Valid, but: ", J4), CONCATENATE("INVALID - FIELD EXCLUDED: ", J4))))</f>
         <v>Valid</v>
       </c>
@@ -3100,11 +3132,11 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>1</v>
@@ -3125,7 +3157,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K5" s="27" t="str">
+      <c r="K5" s="26" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3148,16 +3180,16 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>1</v>
@@ -3179,7 +3211,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K6" s="27" t="str">
+      <c r="K6" s="26" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3202,22 +3234,22 @@
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="6" t="str">
         <f t="array" ref="G7">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
@@ -3235,7 +3267,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K7" s="27" t="str">
+      <c r="K7" s="26" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3269,16 +3301,16 @@
     </row>
     <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>1</v>
@@ -3300,7 +3332,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K8" s="27" t="str">
+      <c r="K8" s="26" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -3334,16 +3366,16 @@
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>3</v>
@@ -3365,7 +3397,7 @@
         <f t="shared" si="1"/>
         <v>Unsupported Field Type Combination</v>
       </c>
-      <c r="K9" s="27" t="str">
+      <c r="K9" s="26" t="str">
         <f t="shared" si="2"/>
         <v>INVALID - FIELD EXCLUDED: Unsupported Field Type Combination</v>
       </c>
@@ -3392,16 +3424,16 @@
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>6</v>
@@ -3423,7 +3455,7 @@
         <f t="shared" si="1"/>
         <v>Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)</v>
       </c>
-      <c r="K10" s="27" t="str">
+      <c r="K10" s="26" t="str">
         <f>IF(H10="", "", IF( J10="", IF( H10="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H10="TRUE", CONCATENATE("Valid, but: ", J10), CONCATENATE("INVALID - FIELD EXCLUDED: ", J10))))</f>
         <v>INVALID - FIELD EXCLUDED: Syncing to Date fields is not yet supported by Zenchimp, use a Text field in Mailchimp or raise a feature request on github :)</v>
       </c>
@@ -3471,7 +3503,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="27" t="str">
+      <c r="K11" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3519,7 +3551,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="27" t="str">
+      <c r="K12" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3567,7 +3599,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="27" t="str">
+      <c r="K13" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3615,7 +3647,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K14" s="27" t="str">
+      <c r="K14" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3663,7 +3695,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="27" t="str">
+      <c r="K15" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3711,7 +3743,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="27" t="str">
+      <c r="K16" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3759,7 +3791,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="27" t="str">
+      <c r="K17" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3807,7 +3839,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K18" s="27" t="str">
+      <c r="K18" s="26" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4882,272 +4914,286 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="26" customWidth="1"/>
-    <col min="2" max="11" width="29" style="26" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="25" customWidth="1"/>
+    <col min="2" max="11" width="29" style="25" customWidth="1"/>
     <col min="12" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24" t="s">
-        <v>65</v>
+      <c r="H2" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="H3" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="24" t="s">
+    <row r="6" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="24" t="s">
+      <c r="C6" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="24" t="s">
+      <c r="H6" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="24" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>75</v>
+      <c r="H8" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="24" t="s">
+    <row r="9" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24" t="s">
-        <v>68</v>
+      <c r="H9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More Improvements to Settings Generator Spreadsheet
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/ZenChimp-Zendesk-App-Mailchimp-Sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB6321-A8D4-E545-89A4-C8B10AFE5B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05945884-1D3B-254C-B09B-4D06D5ED0C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="92">
   <si>
     <t>Zendesk Field Types</t>
   </si>
@@ -310,16 +310,13 @@
   </si>
   <si>
     <t>JHKJHJ</t>
-  </si>
-  <si>
-    <t>ZD_KJH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,8 +427,16 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -482,7 +487,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -637,7 +642,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -677,7 +682,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -721,60 +725,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1149,7 +1106,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1170,19 +1127,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1207,7 +1164,7 @@
       <c r="H2" s="18">
         <v>1</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>71</v>
       </c>
       <c r="J2" s="19">
@@ -1233,13 +1190,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1264,7 +1221,7 @@
         <f t="shared" ref="J3:J17" si="1">TRIM(MID(SUBSTITUTE($G3,"|",REPT(" ",LEN($G3))),(3-1)*LEN($G3)+1,LEN($G3)))</f>
         <v/>
       </c>
-      <c r="K3" s="25" t="str">
+      <c r="K3" s="24" t="str">
         <f t="shared" ref="K3:K17" si="2">IF(H3="", "", IF( J3="", IF( H3="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H3="TRUE", CONCATENATE("Valid, but: ", J3), CONCATENATE("INVALID - FIELD EXCLUDED: ", J3))))</f>
         <v>Valid</v>
       </c>
@@ -1286,9 +1243,9 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
@@ -1311,7 +1268,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K4" s="25" t="str">
+      <c r="K4" s="24" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -1365,7 +1322,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K5" s="25" t="str">
+      <c r="K5" s="24" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -1421,7 +1378,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K6" s="25" t="str">
+      <c r="K6" s="24" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -1486,7 +1443,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K7" s="25" t="str">
+      <c r="K7" s="24" t="str">
         <f t="shared" si="2"/>
         <v>Valid</v>
       </c>
@@ -1541,7 +1498,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K8" s="25" t="str">
+      <c r="K8" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1589,7 +1546,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K9" s="25" t="str">
+      <c r="K9" s="24" t="str">
         <f>IF(H9="", "", IF( J9="", IF( H9="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H9="TRUE", CONCATENATE("Valid, but: ", J9), CONCATENATE("INVALID - FIELD EXCLUDED: ", J9))))</f>
         <v/>
       </c>
@@ -1637,7 +1594,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K10" s="25" t="str">
+      <c r="K10" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1685,7 +1642,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="25" t="str">
+      <c r="K11" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1733,7 +1690,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="25" t="str">
+      <c r="K12" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1781,7 +1738,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="25" t="str">
+      <c r="K13" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1829,7 +1786,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K14" s="25" t="str">
+      <c r="K14" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1877,7 +1834,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="25" t="str">
+      <c r="K15" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1925,7 +1882,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="25" t="str">
+      <c r="K16" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1973,7 +1930,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="25" t="str">
+      <c r="K17" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2005,7 +1962,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="29" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$3, $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$314, $O$15, $O$16, $O$17,"]")</f>
         <v>[
   {
@@ -2024,651 +1981,651 @@
   }
 ]</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="30"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="30"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="30"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
+      <c r="A65" s="29"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
+      <c r="A66" s="29"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
+      <c r="A68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="30"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="30"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
+      <c r="A70" s="29"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="30"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
+      <c r="A71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="30"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="30"/>
+      <c r="A72" s="29"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="30"/>
-      <c r="B73" s="30"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
+      <c r="A73" s="29"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="30"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="30"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="30"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
+      <c r="A76" s="29"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="30"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
+      <c r="A77" s="29"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="30"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="30"/>
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="30"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
+      <c r="A79" s="29"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="30"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="30"/>
-      <c r="F83" s="30"/>
+      <c r="A83" s="29"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="30"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="30"/>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="30"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="30"/>
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="30"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="30"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="30"/>
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="30"/>
-      <c r="B91" s="30"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="30"/>
+      <c r="A91" s="29"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="30"/>
+      <c r="A93" s="29"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="29"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="30"/>
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="30"/>
+      <c r="A96" s="29"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="30"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="30"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="30"/>
-      <c r="F99" s="30"/>
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3580,22 +3537,22 @@
     <mergeCell ref="A3:A4"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:I17 A6:C10 E6:I10">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>AND($C5="", $E5="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3642,7 +3599,7 @@
   <dimension ref="A1:P998"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3664,14 +3621,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -3698,7 +3655,7 @@
       <c r="H2" s="18">
         <v>1</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>71</v>
       </c>
       <c r="J2" s="19">
@@ -3733,13 +3690,11 @@
       <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="5" t="str">
         <f t="array" ref="G3">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C3,Hidden!$A$2:$A$9,0), MATCH($E3,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C3,Hidden!$A$2:$A$9,0), MATCH($E3,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
@@ -3756,7 +3711,7 @@
         <f t="shared" ref="J3:J15" si="2">TRIM(MID(SUBSTITUTE($G3,"|",REPT(" ",LEN($G3))),(3-1)*LEN($G3)+1,LEN($G3)))</f>
         <v/>
       </c>
-      <c r="K3" s="25" t="str">
+      <c r="K3" s="24" t="str">
         <f t="shared" ref="K3:K6" si="3">IF(H3="", "", IF( J3="", IF( H3="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H3="TRUE", CONCATENATE("Valid, but: ", J3), CONCATENATE("INVALID - FIELD EXCLUDED: ", J3))))</f>
         <v>Valid</v>
       </c>
@@ -3812,7 +3767,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K4" s="25" t="str">
+      <c r="K4" s="24" t="str">
         <f t="shared" si="3"/>
         <v>Valid</v>
       </c>
@@ -3877,7 +3832,7 @@
         <f t="shared" si="2"/>
         <v>Please use full, existing URLs when entering values in Zendesk</v>
       </c>
-      <c r="K5" s="25" t="str">
+      <c r="K5" s="24" t="str">
         <f t="shared" si="3"/>
         <v>Valid, but: Please use full, existing URLs when entering values in Zendesk</v>
       </c>
@@ -3942,7 +3897,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K6" s="25" t="str">
+      <c r="K6" s="24" t="str">
         <f t="shared" si="3"/>
         <v>Valid</v>
       </c>
@@ -3997,7 +3952,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K7" s="25" t="str">
+      <c r="K7" s="24" t="str">
         <f>IF(H7="", "", IF( J7="", IF( H7="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H7="TRUE", CONCATENATE("Valid, but: ", J7), CONCATENATE("INVALID - FIELD EXCLUDED: ", J7))))</f>
         <v/>
       </c>
@@ -4045,7 +4000,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K8" s="25" t="str">
+      <c r="K8" s="24" t="str">
         <f t="shared" ref="K8:K15" si="9">IF(H8="", "", IF( J8="", IF( H8="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H8="TRUE", CONCATENATE("Valid, but: ", J8), CONCATENATE("INVALID - FIELD EXCLUDED: ", J8))))</f>
         <v/>
       </c>
@@ -4093,7 +4048,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K9" s="25" t="str">
+      <c r="K9" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4141,7 +4096,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K10" s="25" t="str">
+      <c r="K10" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4189,7 +4144,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="25" t="str">
+      <c r="K11" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4237,7 +4192,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="25" t="str">
+      <c r="K12" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4285,7 +4240,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="25" t="str">
+      <c r="K13" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4333,7 +4288,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="25" t="str">
+      <c r="K14" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4381,7 +4336,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="25" t="str">
+      <c r="K15" s="24" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
@@ -4410,7 +4365,7 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="str">
+      <c r="A17" s="36" t="str">
         <f>CONCATENATE("[",CHAR(10), $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$312, $O$13, $O$14, $O$15,"]")</f>
         <v>[
   {
@@ -4436,668 +4391,668 @@
   }
 ]</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="K17" s="26"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="37"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
+      <c r="A61" s="36"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="36"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="37"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
+      <c r="A63" s="36"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
+      <c r="A64" s="36"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="37"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
+      <c r="A66" s="36"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
+      <c r="A67" s="36"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
+      <c r="A68" s="36"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
+      <c r="A69" s="36"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
+      <c r="A70" s="36"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
+      <c r="A71" s="36"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="37"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
+      <c r="A72" s="36"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
+      <c r="A73" s="36"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
+      <c r="A74" s="36"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="37"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="37"/>
+      <c r="A75" s="36"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
+      <c r="A76" s="36"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="36"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
+      <c r="A77" s="36"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
+      <c r="A78" s="36"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="37"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
+      <c r="A79" s="36"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
+      <c r="A80" s="36"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="36"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="37"/>
+      <c r="A81" s="36"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
+      <c r="A82" s="36"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="36"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="37"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
+      <c r="A84" s="36"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="36"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="37"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
+      <c r="A85" s="36"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="36"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="36"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="37"/>
+      <c r="A86" s="36"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="37"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="36"/>
+      <c r="D87" s="36"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="36"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="37"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
+      <c r="A88" s="36"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="37"/>
+      <c r="A89" s="36"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="36"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
+      <c r="A90" s="36"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="36"/>
+      <c r="D90" s="36"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="36"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="37"/>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
+      <c r="A91" s="36"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="36"/>
+      <c r="F91" s="36"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="37"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="37"/>
+      <c r="A92" s="36"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="36"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="36"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="37"/>
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
+      <c r="A93" s="36"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="36"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="37"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
+      <c r="A94" s="36"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="36"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="36"/>
+      <c r="F94" s="36"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="37"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
+      <c r="A95" s="36"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="36"/>
+      <c r="F95" s="36"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="37"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="37"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="37"/>
+      <c r="A96" s="36"/>
+      <c r="B96" s="36"/>
+      <c r="C96" s="36"/>
+      <c r="D96" s="36"/>
+      <c r="E96" s="36"/>
+      <c r="F96" s="36"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="37"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="37"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
+      <c r="A97" s="36"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="36"/>
+      <c r="E97" s="36"/>
+      <c r="F97" s="36"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="37"/>
-      <c r="B98" s="37"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="37"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="37"/>
+      <c r="A98" s="36"/>
+      <c r="B98" s="36"/>
+      <c r="C98" s="36"/>
+      <c r="D98" s="36"/>
+      <c r="E98" s="36"/>
+      <c r="F98" s="36"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="37"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
+      <c r="A99" s="36"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="36"/>
+      <c r="D99" s="36"/>
+      <c r="E99" s="36"/>
+      <c r="F99" s="36"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6004,22 +5959,22 @@
     <mergeCell ref="A17:F99"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I15">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND($C3="", $E3="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6070,25 +6025,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="26" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="26" customWidth="1"/>
-    <col min="4" max="5" width="15.5703125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="115.5703125" style="26" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="26" customWidth="1"/>
-    <col min="9" max="18" width="10.5703125" style="26" customWidth="1"/>
-    <col min="19" max="16384" width="11.28515625" style="26"/>
+    <col min="1" max="1" width="26.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="25" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="115.5703125" style="25" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" style="25" customWidth="1"/>
+    <col min="9" max="18" width="10.5703125" style="25" customWidth="1"/>
+    <col min="19" max="16384" width="11.28515625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -6132,7 +6087,7 @@
       <c r="E3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="25" t="str">
+      <c r="F3" s="24" t="str">
         <f>IF(OR(C3="", B3=""), "", IF(AND($D3="", $E3=""), "INVALID - FIELD EXCLUDED: Please enter a value for when the checkbox is ticked and unticked", IF(AND($C3&lt;&gt;"Text", $C3&lt;&gt;"Number", $C3&lt;&gt;"Radio Buttons", $C3&lt;&gt;"Drop Down"), "INVALID - FIELD EXCLUDED: Field type "&amp;$C3&amp;" not yet supported in Zenchimp for Mailchimp only fields, please use another field type or raise a feature request on GitHub :)", "Valid, but please make sure your 2 values are valid for field type '"&amp;$C3&amp;"'" &amp; IF(OR($D3="", $E3="")," and please make sure your Mailchimp field '"&amp;$B3&amp;"' is not marked as 'Required' as one of your values is blank","") ) ) )</f>
         <v>Valid, but please make sure your 2 values are valid for field type 'Radio Buttons'</v>
       </c>
@@ -6164,7 +6119,7 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="25" t="str">
+      <c r="F4" s="24" t="str">
         <f t="shared" ref="F4:F15" si="1">IF(OR(C4="", B4=""), "", IF(AND($D4="", $E4=""), "INVALID - FIELD EXCLUDED: Please enter a value for when the checkbox is ticked and unticked", IF(AND($C4&lt;&gt;"Text", $C4&lt;&gt;"Number", $C4&lt;&gt;"Radio Buttons", $C4&lt;&gt;"Drop Down"), "INVALID - FIELD EXCLUDED: Field type "&amp;$C4&amp;" not yet supported in Zenchimp for Mailchimp only fields, please use another field type or raise a feature request on GitHub :)", "Valid, but please make sure your values are valid for field type '"&amp;$C4&amp;"'" &amp; IF(OR($D4="", $E4="")," and please make sure your Mailchimp field '"&amp;$B4&amp;"' is not marked as 'Required' as one of your values is blank","") ) ) )</f>
         <v>INVALID - FIELD EXCLUDED: Please enter a value for when the checkbox is ticked and unticked</v>
       </c>
@@ -6190,7 +6145,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="25" t="str">
+      <c r="F5" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6209,7 +6164,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="25" t="str">
+      <c r="F6" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6228,7 +6183,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="25" t="str">
+      <c r="F7" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6247,7 +6202,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="25" t="str">
+      <c r="F8" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6266,7 +6221,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="25" t="str">
+      <c r="F9" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6285,7 +6240,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="25" t="str">
+      <c r="F10" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6304,7 +6259,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="25" t="str">
+      <c r="F11" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6323,7 +6278,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="25" t="str">
+      <c r="F12" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6342,7 +6297,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="25" t="str">
+      <c r="F13" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6361,7 +6316,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="25" t="str">
+      <c r="F14" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6380,7 +6335,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="25" t="str">
+      <c r="F15" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -6397,7 +6352,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="str">
+      <c r="A17" s="36" t="str">
         <f>CONCATENATE("[",CHAR(10), $G$3,$G$4, $G$5, $G$6, $G$7, $G$8, $G$9, $G$10, $G$11, $G$312, $G$13, $G$14, $G$15,"]")</f>
         <v>[
   {
@@ -6416,584 +6371,584 @@
   }
 ]</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="37"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="37"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="36"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="37"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="36"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="37"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="36"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="37"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="36"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="37"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="36"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="37"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="36"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="37"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="37"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="37"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="36"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="37"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="36"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="37"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="36"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="37"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="37"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="37"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="36"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="37"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="36"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="37"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="37"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="37"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="36"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="37"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="37"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="36"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="37"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="36"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="37"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="36"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="37"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="36"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="37"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="36"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="37"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="37"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="36"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="37"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="36"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="37"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="37"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="37"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="36"/>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="37"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="37"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="36"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="37"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="36"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="37"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="36"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="37"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="36"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="37"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="37"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="37"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="37"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="36"/>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="37"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="36"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="37"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="37"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="36"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="37"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="36"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="37"/>
+      <c r="A61" s="36"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="36"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="37"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="37"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="36"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="37"/>
+      <c r="A63" s="36"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="36"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="37"/>
+      <c r="A64" s="36"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="36"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="37"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="36"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="37"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="37"/>
+      <c r="A66" s="36"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="36"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="37"/>
+      <c r="A67" s="36"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="36"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="37"/>
+      <c r="A68" s="36"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="36"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="37"/>
+      <c r="A69" s="36"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="36"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="37"/>
+      <c r="A70" s="36"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="36"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="37"/>
+      <c r="A71" s="36"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="36"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="37"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="37"/>
+      <c r="A72" s="36"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="36"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="37"/>
+      <c r="A73" s="36"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="36"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="37"/>
+      <c r="A74" s="36"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="36"/>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="37"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="37"/>
+      <c r="A75" s="36"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="36"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="37"/>
+      <c r="A76" s="36"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="36"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="37"/>
+      <c r="A77" s="36"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="36"/>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="37"/>
+      <c r="A78" s="36"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="36"/>
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="37"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="37"/>
+      <c r="A79" s="36"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="36"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="37"/>
+      <c r="A80" s="36"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="36"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="37"/>
+      <c r="A81" s="36"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="36"/>
     </row>
     <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="37"/>
+      <c r="A82" s="36"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="36"/>
     </row>
     <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="37"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="37"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="36"/>
     </row>
     <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="37"/>
+      <c r="A84" s="36"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="36"/>
     </row>
     <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="37"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="37"/>
+      <c r="A85" s="36"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="36"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="37"/>
+      <c r="A86" s="36"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="36"/>
     </row>
     <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="37"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="37"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="36"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="36"/>
     </row>
     <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="37"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="37"/>
+      <c r="A88" s="36"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="36"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="37"/>
+      <c r="A89" s="36"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="36"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="37"/>
+      <c r="A90" s="36"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="36"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="36"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="37"/>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="37"/>
+      <c r="A91" s="36"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="36"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="37"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="37"/>
+      <c r="A92" s="36"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="36"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="36"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="37"/>
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="37"/>
+      <c r="A93" s="36"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="36"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="36"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="37"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="37"/>
+      <c r="A94" s="36"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="36"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="36"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="37"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="37"/>
+      <c r="A95" s="36"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="36"/>
     </row>
     <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="37"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="37"/>
+      <c r="A96" s="36"/>
+      <c r="B96" s="36"/>
+      <c r="C96" s="36"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="36"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="37"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="37"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="37"/>
+      <c r="A97" s="36"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="36"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="37"/>
-      <c r="B98" s="37"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="37"/>
+      <c r="A98" s="36"/>
+      <c r="B98" s="36"/>
+      <c r="C98" s="36"/>
+      <c r="D98" s="37"/>
+      <c r="E98" s="36"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="37"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="37"/>
+      <c r="A99" s="36"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="36"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="36"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7900,17 +7855,17 @@
     <mergeCell ref="A17:E99"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F15">
-    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="Valid">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="Valid">
       <formula>LEFT(F3,LEN("Valid"))="Valid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F15">
-    <cfRule type="beginsWith" dxfId="3" priority="4" operator="beginsWith" text="INVALID">
+    <cfRule type="beginsWith" dxfId="1" priority="4" operator="beginsWith" text="INVALID">
       <formula>LEFT(F3,LEN("INVALID"))="INVALID"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:E15">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>AND($B2="", $C2="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7955,293 +7910,293 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="24" customWidth="1"/>
-    <col min="2" max="11" width="29" style="24" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="23" customWidth="1"/>
+    <col min="2" max="11" width="29" style="23" customWidth="1"/>
     <col min="12" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22" t="s">
+      <c r="I5" s="21"/>
+      <c r="J5" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="21" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22" t="s">
+      <c r="I8" s="21"/>
+      <c r="J8" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="21" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="21"/>
+      <c r="J9" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="21" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished Porting (v2.0.1) It works, but want to test more before release however
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/ZenChimp-Zendesk-App-Mailchimp-Sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05945884-1D3B-254C-B09B-4D06D5ED0C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547A30AC-1922-7F41-8BC6-6789B4BEA5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
   <si>
     <t>Zendesk Field Types</t>
   </si>
@@ -159,9 +159,6 @@
     <t>SITES_LIST</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Mailchimp Footer Message</t>
   </si>
   <si>
@@ -273,18 +270,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>Weekly Newsletter</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>My Checkbox</t>
-  </si>
-  <si>
-    <t>NEWSLETTER</t>
-  </si>
-  <si>
     <t>Mailchimp Default Value</t>
   </si>
   <si>
@@ -309,7 +297,22 @@
     <t>TRUE|text|Please use a regular expressuin that forces full,  URLs in Zendesk|||</t>
   </si>
   <si>
-    <t>JHKJHJ</t>
+    <t>SEND_MAINT</t>
+  </si>
+  <si>
+    <t>Maintenance Emails</t>
+  </si>
+  <si>
+    <t>SEND_PROMO</t>
+  </si>
+  <si>
+    <t>VIP Promotion Emails</t>
+  </si>
+  <si>
+    <t>SEND_SC</t>
+  </si>
+  <si>
+    <t>Monthly Scorecard Emails</t>
   </si>
 </sst>
 </file>
@@ -700,6 +703,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -725,13 +729,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -764,6 +767,17 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -821,6 +835,52 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFEB9C"/>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1" tint="0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1127,14 +1187,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="A1" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="27"/>
@@ -1158,14 +1218,14 @@
         <v>29</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="18">
         <v>1</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" s="19">
         <v>3</v>
@@ -1190,13 +1250,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="A3" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1243,9 +1303,9 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
@@ -1359,9 +1419,7 @@
       <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="5" t="str">
         <f t="array" ref="G6">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C6,Hidden!$A$2:$A$9,0), MATCH($E6,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C6,Hidden!$A$2:$A$9,0), MATCH($E6,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
@@ -1401,7 +1459,7 @@
     "zendesk_field" : "site_list",
     "mailchimp_field" : "SITES_LIST",
     "type" : "text",
-    "default_value" : "None"
+    "default_value" : ""
   },
 </v>
       </c>
@@ -1412,16 +1470,16 @@
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>1</v>
@@ -1962,7 +2020,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="str">
+      <c r="A19" s="30" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$3, $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$314, $O$15, $O$16, $O$17,"]")</f>
         <v>[
   {
@@ -1970,7 +2028,7 @@
     "zendesk_field" : "site_list",
     "mailchimp_field" : "SITES_LIST",
     "type" : "text",
-    "default_value" : "None"
+    "default_value" : ""
   },
   {
     "field_label" : "Mailchimp Footer Message",
@@ -1981,651 +2039,651 @@
   }
 ]</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="29"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="29"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="29"/>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="29"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="29"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="29"/>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="29"/>
-      <c r="B64" s="29"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="29"/>
-      <c r="B65" s="29"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="29"/>
-      <c r="B66" s="29"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="29"/>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="29"/>
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
-      <c r="B69" s="29"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="29"/>
-      <c r="B70" s="29"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="29"/>
-      <c r="B71" s="29"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="29"/>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="29"/>
-      <c r="B72" s="29"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="29"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
+      <c r="A72" s="30"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="29"/>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="29"/>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="30"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="29"/>
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="29"/>
-      <c r="B76" s="29"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="29"/>
-      <c r="F76" s="29"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="29"/>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="30"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="29"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="30"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="29"/>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="30"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="29"/>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="30"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="29"/>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="29"/>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="30"/>
+      <c r="F82" s="30"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="29"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
+      <c r="A83" s="30"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="30"/>
+      <c r="F83" s="30"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="29"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
+      <c r="A84" s="30"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="30"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="29"/>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
+      <c r="A85" s="30"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="29"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
+      <c r="A86" s="30"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="30"/>
+      <c r="F86" s="30"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="29"/>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
+      <c r="A87" s="30"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="29"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
+      <c r="A88" s="30"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="30"/>
+      <c r="F88" s="30"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="29"/>
-      <c r="B89" s="29"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="29"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
+      <c r="A89" s="30"/>
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="30"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="29"/>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="30"/>
+      <c r="F90" s="30"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="29"/>
-      <c r="B91" s="29"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
+      <c r="A91" s="30"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="30"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="29"/>
-      <c r="B92" s="29"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
+      <c r="A92" s="30"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="30"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="29"/>
-      <c r="B93" s="29"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="29"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="29"/>
+      <c r="A93" s="30"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="30"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="29"/>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
+      <c r="A94" s="30"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="30"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="29"/>
-      <c r="B95" s="29"/>
-      <c r="C95" s="29"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
+      <c r="A95" s="30"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="30"/>
+      <c r="E95" s="30"/>
+      <c r="F95" s="30"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="29"/>
-      <c r="B96" s="29"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="29"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
+      <c r="A96" s="30"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="30"/>
+      <c r="F96" s="30"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="29"/>
-      <c r="B97" s="29"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
+      <c r="A97" s="30"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="30"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="29"/>
-      <c r="B98" s="29"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
+      <c r="A98" s="30"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="30"/>
+      <c r="F98" s="30"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="29"/>
-      <c r="B99" s="29"/>
-      <c r="C99" s="29"/>
-      <c r="D99" s="29"/>
-      <c r="E99" s="29"/>
-      <c r="F99" s="29"/>
+      <c r="A99" s="30"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="30"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3537,22 +3595,22 @@
     <mergeCell ref="A3:A4"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:I17 A6:C10 E6:I10">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="A6:F17">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND($C5="", $E5="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3599,7 +3657,7 @@
   <dimension ref="A1:P998"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3621,14 +3679,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="A1" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -3649,14 +3707,14 @@
         <v>29</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="18">
         <v>1</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" s="19">
         <v>3</v>
@@ -3682,19 +3740,19 @@
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="38"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="5" t="str">
         <f t="array" ref="G3">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C3,Hidden!$A$2:$A$9,0), MATCH($E3,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C3,Hidden!$A$2:$A$9,0), MATCH($E3,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
         <v>TRUE|text</v>
@@ -3734,22 +3792,22 @@
     </row>
     <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="5" t="str">
         <f t="array" ref="G4">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C4,Hidden!$A$2:$A$9,0), MATCH($E4,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C4,Hidden!$A$2:$A$9,0), MATCH($E4,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
@@ -3801,16 +3859,16 @@
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>10</v>
@@ -3866,16 +3924,16 @@
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
@@ -4365,7 +4423,7 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="str">
+      <c r="A17" s="37" t="str">
         <f>CONCATENATE("[",CHAR(10), $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$312, $O$13, $O$14, $O$15,"]")</f>
         <v>[
   {
@@ -4391,668 +4449,668 @@
   }
 ]</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="K17" s="25"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="36"/>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="36"/>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="36"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="36"/>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="36"/>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="36"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="36"/>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="36"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="36"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="36"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="36"/>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="36"/>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="36"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="36"/>
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="36"/>
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="36"/>
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="36"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="36"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="36"/>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="36"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="36"/>
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="36"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="36"/>
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="36"/>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="36"/>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="36"/>
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="36"/>
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="36"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="36"/>
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="36"/>
-      <c r="B89" s="36"/>
-      <c r="C89" s="36"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="36"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="37"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="36"/>
-      <c r="B90" s="36"/>
-      <c r="C90" s="36"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36"/>
-      <c r="F90" s="36"/>
+      <c r="A90" s="37"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="36"/>
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
-      <c r="F91" s="36"/>
+      <c r="A91" s="37"/>
+      <c r="B91" s="37"/>
+      <c r="C91" s="37"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="37"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="36"/>
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
-      <c r="F92" s="36"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="36"/>
-      <c r="B93" s="36"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
-      <c r="F93" s="36"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="36"/>
-      <c r="B94" s="36"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="36"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="36"/>
-      <c r="B95" s="36"/>
-      <c r="C95" s="36"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
-      <c r="F95" s="36"/>
+      <c r="A95" s="37"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="36"/>
-      <c r="B96" s="36"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="36"/>
-      <c r="F96" s="36"/>
+      <c r="A96" s="37"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="37"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="36"/>
-      <c r="B97" s="36"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
-      <c r="F97" s="36"/>
+      <c r="A97" s="37"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="37"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="36"/>
-      <c r="B98" s="36"/>
-      <c r="C98" s="36"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="36"/>
+      <c r="A98" s="37"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="37"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="37"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="36"/>
-      <c r="B99" s="36"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="36"/>
+      <c r="A99" s="37"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="37"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5959,22 +6017,22 @@
     <mergeCell ref="A17:F99"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I15">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND($C3="", $E3="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6020,7 +6078,7 @@
   <dimension ref="A1:H998"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A17" sqref="A17:E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6036,13 +6094,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6056,10 +6114,10 @@
         <v>29</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>74</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>75</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>30</v>
@@ -6073,19 +6131,19 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="F3" s="24" t="str">
         <f>IF(OR(C3="", B3=""), "", IF(AND($D3="", $E3=""), "INVALID - FIELD EXCLUDED: Please enter a value for when the checkbox is ticked and unticked", IF(AND($C3&lt;&gt;"Text", $C3&lt;&gt;"Number", $C3&lt;&gt;"Radio Buttons", $C3&lt;&gt;"Drop Down"), "INVALID - FIELD EXCLUDED: Field type "&amp;$C3&amp;" not yet supported in Zenchimp for Mailchimp only fields, please use another field type or raise a feature request on GitHub :)", "Valid, but please make sure your 2 values are valid for field type '"&amp;$C3&amp;"'" &amp; IF(OR($D3="", $E3="")," and please make sure your Mailchimp field '"&amp;$B3&amp;"' is not marked as 'Required' as one of your values is blank","") ) ) )</f>
@@ -6094,8 +6152,8 @@
       <c r="G3" s="1" t="str">
         <f>IF($F3&lt;&gt;"", "  {"&amp;CHAR(10)&amp;"    ""field_label"" : """&amp;$A3&amp;""","&amp;CHAR(10)&amp;"    ""mailchimp_field"" : """&amp;$B3&amp;""","&amp;CHAR(10)&amp;"    ""type"" : ""checkbox"","&amp;CHAR(10)&amp;"    ""value_if_ticked"" : """&amp;$D3&amp;""","&amp;CHAR(10)&amp;"    ""value_if_unticked"" : """&amp;$E3&amp;""""&amp;CHAR(10)&amp;"  }"&amp;$H3&amp;CHAR(10),  "")</f>
         <v xml:space="preserve">  {
-    "field_label" : "Weekly Newsletter",
-    "mailchimp_field" : "NEWSLETTER",
+    "field_label" : "Maintenance Emails",
+    "mailchimp_field" : "SEND_MAINT",
     "type" : "checkbox",
     "value_if_ticked" : "Yes",
     "value_if_unticked" : "No"
@@ -6109,49 +6167,68 @@
     </row>
     <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
       <c r="F4" s="24" t="str">
         <f t="shared" ref="F4:F15" si="1">IF(OR(C4="", B4=""), "", IF(AND($D4="", $E4=""), "INVALID - FIELD EXCLUDED: Please enter a value for when the checkbox is ticked and unticked", IF(AND($C4&lt;&gt;"Text", $C4&lt;&gt;"Number", $C4&lt;&gt;"Radio Buttons", $C4&lt;&gt;"Drop Down"), "INVALID - FIELD EXCLUDED: Field type "&amp;$C4&amp;" not yet supported in Zenchimp for Mailchimp only fields, please use another field type or raise a feature request on GitHub :)", "Valid, but please make sure your values are valid for field type '"&amp;$C4&amp;"'" &amp; IF(OR($D4="", $E4="")," and please make sure your Mailchimp field '"&amp;$B4&amp;"' is not marked as 'Required' as one of your values is blank","") ) ) )</f>
-        <v>INVALID - FIELD EXCLUDED: Please enter a value for when the checkbox is ticked and unticked</v>
+        <v>Valid, but please make sure your values are valid for field type 'Number'</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ref="G4:G15" si="2">IF($F4&lt;&gt;"", "  {"&amp;CHAR(10)&amp;"    ""field_label"" : """&amp;$A4&amp;""","&amp;CHAR(10)&amp;"    ""mailchimp_field"" : """&amp;$B4&amp;""","&amp;CHAR(10)&amp;"    ""type"" : ""checkbox"","&amp;CHAR(10)&amp;"    ""value_if_ticked"" : """&amp;$D4&amp;""","&amp;CHAR(10)&amp;"    ""value_if_unticked"" : """&amp;$E4&amp;""""&amp;CHAR(10)&amp;"  }"&amp;$H4&amp;CHAR(10),  "")</f>
         <v xml:space="preserve">  {
-    "field_label" : "My Checkbox",
-    "mailchimp_field" : "JHKJHJ",
+    "field_label" : "VIP Promotion Emails",
+    "mailchimp_field" : "SEND_PROMO",
     "type" : "checkbox",
-    "value_if_ticked" : "",
+    "value_if_ticked" : "1",
+    "value_if_unticked" : "0"
+  },
+</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>Valid, but please make sure your values are valid for field type 'Text' and please make sure your Mailchimp field 'SEND_SC' is not marked as 'Required' as one of your values is blank</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  {
+    "field_label" : "Monthly Scorecard Emails",
+    "mailchimp_field" : "SEND_SC",
+    "type" : "checkbox",
+    "value_if_ticked" : "0",
     "value_if_unticked" : ""
   }
 </v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6352,603 +6429,610 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="str">
+      <c r="A17" s="37" t="str">
         <f>CONCATENATE("[",CHAR(10), $G$3,$G$4, $G$5, $G$6, $G$7, $G$8, $G$9, $G$10, $G$11, $G$312, $G$13, $G$14, $G$15,"]")</f>
         <v>[
   {
-    "field_label" : "Weekly Newsletter",
-    "mailchimp_field" : "NEWSLETTER",
+    "field_label" : "Maintenance Emails",
+    "mailchimp_field" : "SEND_MAINT",
     "type" : "checkbox",
     "value_if_ticked" : "Yes",
     "value_if_unticked" : "No"
   },
   {
-    "field_label" : "My Checkbox",
-    "mailchimp_field" : "JHKJHJ",
+    "field_label" : "VIP Promotion Emails",
+    "mailchimp_field" : "SEND_PROMO",
     "type" : "checkbox",
-    "value_if_ticked" : "",
+    "value_if_ticked" : "1",
+    "value_if_unticked" : "0"
+  },
+  {
+    "field_label" : "Monthly Scorecard Emails",
+    "mailchimp_field" : "SEND_SC",
+    "type" : "checkbox",
+    "value_if_ticked" : "0",
     "value_if_unticked" : ""
   }
 ]</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="36"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="36"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="36"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="36"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="37"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="36"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="37"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="36"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="37"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="36"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="37"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="36"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="37"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="36"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="37"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="36"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="37"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="36"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="37"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="36"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="37"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="36"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="37"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="36"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="37"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="36"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="37"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="36"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="36"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="37"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="36"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="37"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="36"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="37"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="36"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="37"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="36"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="37"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="36"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="37"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="36"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="37"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="36"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="37"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="36"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="36"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="37"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="36"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="37"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="36"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="37"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="36"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="37"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="36"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="37"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="36"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="37"/>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="36"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="37"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="36"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="37"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="36"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="37"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="36"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="37"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="36"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="37"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="36"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="37"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="36"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="37"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="36"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="37"/>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="36"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="37"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="36"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="37"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="36"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="37"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="36"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="37"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="36"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="37"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="36"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="37"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="36"/>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="36"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="37"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="36"/>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="36"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="37"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="36"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="36"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="37"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="36"/>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="36"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="37"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="36"/>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="36"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="37"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="36"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="36"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="37"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="36"/>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="36"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="37"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="36"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="37"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="36"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="36"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="37"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="36"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="36"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="37"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="36"/>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="36"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="37"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="36"/>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="36"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="37"/>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="36"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="36"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="37"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="36"/>
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="36"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="37"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="36"/>
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="36"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="37"/>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="36"/>
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="36"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="37"/>
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="36"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="36"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="37"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="36"/>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="36"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="37"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="36"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="37"/>
     </row>
     <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="36"/>
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="36"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="37"/>
     </row>
     <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="36"/>
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="36"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="37"/>
     </row>
     <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="36"/>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="36"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="37"/>
     </row>
     <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="36"/>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="36"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="37"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="36"/>
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="36"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="37"/>
     </row>
     <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="36"/>
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="36"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="37"/>
     </row>
     <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="36"/>
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="36"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="37"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="36"/>
-      <c r="B89" s="36"/>
-      <c r="C89" s="36"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="36"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="37"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="36"/>
-      <c r="B90" s="36"/>
-      <c r="C90" s="36"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="36"/>
+      <c r="A90" s="37"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="37"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="36"/>
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="36"/>
+      <c r="A91" s="37"/>
+      <c r="B91" s="37"/>
+      <c r="C91" s="37"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="37"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="36"/>
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="36"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="37"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="36"/>
-      <c r="B93" s="36"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="36"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="37"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="36"/>
-      <c r="B94" s="36"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="36"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="38"/>
+      <c r="E94" s="37"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="36"/>
-      <c r="B95" s="36"/>
-      <c r="C95" s="36"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="36"/>
+      <c r="A95" s="37"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="37"/>
     </row>
     <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="36"/>
-      <c r="B96" s="36"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="37"/>
-      <c r="E96" s="36"/>
+      <c r="A96" s="37"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="38"/>
+      <c r="E96" s="37"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="36"/>
-      <c r="B97" s="36"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="36"/>
+      <c r="A97" s="37"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="38"/>
+      <c r="E97" s="37"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="36"/>
-      <c r="B98" s="36"/>
-      <c r="C98" s="36"/>
-      <c r="D98" s="37"/>
-      <c r="E98" s="36"/>
+      <c r="A98" s="37"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="38"/>
+      <c r="E98" s="37"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="36"/>
-      <c r="B99" s="36"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="36"/>
+      <c r="A99" s="37"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="38"/>
+      <c r="E99" s="37"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7855,17 +7939,17 @@
     <mergeCell ref="A17:E99"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F15">
-    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="Valid">
+    <cfRule type="beginsWith" dxfId="10" priority="2" operator="beginsWith" text="Valid">
       <formula>LEFT(F3,LEN("Valid"))="Valid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F15">
-    <cfRule type="beginsWith" dxfId="1" priority="4" operator="beginsWith" text="INVALID">
+    <cfRule type="beginsWith" dxfId="9" priority="4" operator="beginsWith" text="INVALID">
       <formula>LEFT(F3,LEN("INVALID"))="INVALID"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:E15">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>AND($B2="", $C2="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7958,13 +8042,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>13</v>
@@ -7973,14 +8057,14 @@
         <v>13</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="21"/>
       <c r="J2" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -7991,7 +8075,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>14</v>
@@ -8006,14 +8090,14 @@
         <v>13</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -8039,7 +8123,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>19</v>
@@ -8048,7 +8132,7 @@
         <v>20</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -8059,7 +8143,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -8070,14 +8154,14 @@
         <v>13</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -8088,7 +8172,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
@@ -8099,14 +8183,14 @@
         <v>13</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
@@ -8117,13 +8201,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>13</v>
@@ -8132,16 +8216,16 @@
         <v>13</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="K7" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -8152,7 +8236,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
@@ -8163,14 +8247,14 @@
         <v>13</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -8190,14 +8274,14 @@
         <v>13</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Fix - Syncing number --> Text used to show out of sync regardless
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/ZenChimp-Zendesk-App-Mailchimp-Sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547A30AC-1922-7F41-8BC6-6789B4BEA5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337758AE-265F-E340-921B-483A522F6983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zendesk User Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Zendesk Organisation Fields" sheetId="4" r:id="rId2"/>
     <sheet name="Mailchimp Only Fields" sheetId="6" r:id="rId3"/>
-    <sheet name="Hidden" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Generated Settings" sheetId="7" r:id="rId4"/>
+    <sheet name="Hidden" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
   <si>
     <t>Zendesk Field Types</t>
   </si>
@@ -313,17 +314,51 @@
   </si>
   <si>
     <t>Monthly Scorecard Emails</t>
+  </si>
+  <si>
+    <t>Year Customer Joined?</t>
+  </si>
+  <si>
+    <t>STARTYEAR</t>
+  </si>
+  <si>
+    <t>year_customer_joined_us</t>
+  </si>
+  <si>
+    <t>Mailchimp Tag Name of First Name merge field*</t>
+  </si>
+  <si>
+    <t>Mailchimp Tag Name of Last Name name merge field*</t>
+  </si>
+  <si>
+    <t>Mailchimp Tag Name of Customer Type merge field*</t>
+  </si>
+  <si>
+    <t>Zendesk &lt;-&gt; Mailchimp Field Mapping for User fields*</t>
+  </si>
+  <si>
+    <t>Zendesk &lt;-&gt; Mailchimp Field Mapping for Organization fields*</t>
+  </si>
+  <si>
+    <t>Field Definitions for Mailchimp only fields*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -334,12 +369,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -444,8 +473,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF555555"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF68737D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF555555"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,8 +559,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -642,15 +714,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -685,10 +773,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -704,9 +792,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -723,18 +808,37 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -767,17 +871,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -835,52 +928,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFEB9C"/>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1165,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1187,14 +1234,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="27"/>
@@ -1250,13 +1297,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1303,9 +1350,9 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
@@ -2020,7 +2067,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="43" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$3, $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$314, $O$15, $O$16, $O$17,"]")</f>
         <v>[
   {
@@ -2039,651 +2086,651 @@
   }
 ]</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="A48" s="43"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
+      <c r="A49" s="43"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
+      <c r="A50" s="43"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="30"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
+      <c r="A51" s="43"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
+      <c r="A52" s="43"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
+      <c r="A53" s="43"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
+      <c r="A55" s="43"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="30"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
+      <c r="A64" s="43"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="30"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
+      <c r="A68" s="43"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="30"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
+      <c r="A69" s="43"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="43"/>
+      <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="30"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="30"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="30"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="30"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="30"/>
-      <c r="B73" s="30"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="30"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="30"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="30"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="30"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="43"/>
+      <c r="F77" s="43"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="30"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="30"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="30"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
+      <c r="A79" s="43"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="43"/>
+      <c r="D79" s="43"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
+      <c r="A80" s="43"/>
+      <c r="B80" s="43"/>
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="43"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
+      <c r="A81" s="43"/>
+      <c r="B81" s="43"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="43"/>
+      <c r="F81" s="43"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
+      <c r="A82" s="43"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="30"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="30"/>
-      <c r="F83" s="30"/>
+      <c r="A83" s="43"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="43"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="30"/>
+      <c r="A84" s="43"/>
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="30"/>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="30"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="43"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="43"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="30"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="30"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="43"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="30"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="43"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="30"/>
+      <c r="A89" s="43"/>
+      <c r="B89" s="43"/>
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="E89" s="43"/>
+      <c r="F89" s="43"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
+      <c r="A90" s="43"/>
+      <c r="B90" s="43"/>
+      <c r="C90" s="43"/>
+      <c r="D90" s="43"/>
+      <c r="E90" s="43"/>
+      <c r="F90" s="43"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="30"/>
-      <c r="B91" s="30"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="30"/>
+      <c r="A91" s="43"/>
+      <c r="B91" s="43"/>
+      <c r="C91" s="43"/>
+      <c r="D91" s="43"/>
+      <c r="E91" s="43"/>
+      <c r="F91" s="43"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
+      <c r="A92" s="43"/>
+      <c r="B92" s="43"/>
+      <c r="C92" s="43"/>
+      <c r="D92" s="43"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="43"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="30"/>
+      <c r="A93" s="43"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43"/>
+      <c r="F93" s="43"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
+      <c r="A94" s="43"/>
+      <c r="B94" s="43"/>
+      <c r="C94" s="43"/>
+      <c r="D94" s="43"/>
+      <c r="E94" s="43"/>
+      <c r="F94" s="43"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="30"/>
+      <c r="A95" s="43"/>
+      <c r="B95" s="43"/>
+      <c r="C95" s="43"/>
+      <c r="D95" s="43"/>
+      <c r="E95" s="43"/>
+      <c r="F95" s="43"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="30"/>
+      <c r="A96" s="43"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="43"/>
+      <c r="D96" s="43"/>
+      <c r="E96" s="43"/>
+      <c r="F96" s="43"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
+      <c r="A97" s="43"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="43"/>
+      <c r="D97" s="43"/>
+      <c r="E97" s="43"/>
+      <c r="F97" s="43"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="30"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
+      <c r="A98" s="43"/>
+      <c r="B98" s="43"/>
+      <c r="C98" s="43"/>
+      <c r="D98" s="43"/>
+      <c r="E98" s="43"/>
+      <c r="F98" s="43"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="30"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="30"/>
-      <c r="F99" s="30"/>
+      <c r="A99" s="43"/>
+      <c r="B99" s="43"/>
+      <c r="C99" s="43"/>
+      <c r="D99" s="43"/>
+      <c r="E99" s="43"/>
+      <c r="F99" s="43"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3595,22 +3642,22 @@
     <mergeCell ref="A3:A4"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:F17">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>AND($C5="", $E5="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3657,7 +3704,7 @@
   <dimension ref="A1:P998"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A17" sqref="A17:F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3679,14 +3726,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -3979,32 +4026,42 @@
     "mailchimp_field" : "EMPLOYEES",
     "type" : "text",
     "default_value" : ""
-  }
+  },
 </v>
       </c>
       <c r="P6" s="1" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="5" t="str">
         <f t="array" ref="G7">IF( IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) ="", "FALSE||Unsupported Field Type Combination|||", IFERROR(INDEX(Hidden!$B$2:$K$9, MATCH($C7,Hidden!$A$2:$A$9,0), MATCH($E7,Hidden!$B$1:$K$1,0)), "|||||" ) )</f>
-        <v>|||||</v>
+        <v>TRUE|text||||</v>
       </c>
       <c r="H7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>TRUE</v>
       </c>
       <c r="I7" s="13" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>text</v>
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4012,7 +4069,7 @@
       </c>
       <c r="K7" s="24" t="str">
         <f>IF(H7="", "", IF( J7="", IF( H7="TRUE", "Valid", "INVALID - FIELD EXCLUDED: Invalid Data Type Combination"), IF( H7="TRUE", CONCATENATE("Valid, but: ", J7), CONCATENATE("INVALID - FIELD EXCLUDED: ", J7))))</f>
-        <v/>
+        <v>Valid</v>
       </c>
       <c r="L7" s="1" t="str">
         <f t="shared" si="4"/>
@@ -4028,7 +4085,14 @@
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v xml:space="preserve">  {
+    "field_label" : "Year Customer Joined?",
+    "zendesk_field" : "year_customer_joined_us",
+    "mailchimp_field" : "STARTYEAR",
+    "type" : "text",
+    "default_value" : ""
+  }
+</v>
       </c>
       <c r="P7" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4423,7 +4487,7 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="str">
+      <c r="A17" s="44" t="str">
         <f>CONCATENATE("[",CHAR(10), $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$312, $O$13, $O$14, $O$15,"]")</f>
         <v>[
   {
@@ -4446,671 +4510,678 @@
     "mailchimp_field" : "EMPLOYEES",
     "type" : "text",
     "default_value" : ""
+  },
+  {
+    "field_label" : "Year Customer Joined?",
+    "zendesk_field" : "year_customer_joined_us",
+    "mailchimp_field" : "STARTYEAR",
+    "type" : "text",
+    "default_value" : ""
   }
 ]</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
       <c r="K17" s="25"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="37"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="37"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="37"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="44"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="44"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
+      <c r="A69" s="44"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="44"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
+      <c r="A70" s="44"/>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
+      <c r="A71" s="44"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="37"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
+      <c r="A73" s="44"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="44"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="37"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="37"/>
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="44"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="37"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
+      <c r="A79" s="44"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
+      <c r="A80" s="44"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="37"/>
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="37"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="37"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="37"/>
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="37"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="37"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="37"/>
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="37"/>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="37"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="37"/>
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="37"/>
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
+      <c r="A93" s="44"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="37"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="37"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="37"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="37"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="37"/>
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="44"/>
+      <c r="F96" s="44"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="37"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="37"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="37"/>
-      <c r="B98" s="37"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="37"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="37"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="37"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="44"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6017,22 +6088,22 @@
     <mergeCell ref="A17:F99"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I15">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND($C3="", $E3="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6094,13 +6165,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6429,7 +6500,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="str">
+      <c r="A17" s="44" t="str">
         <f>CONCATENATE("[",CHAR(10), $G$3,$G$4, $G$5, $G$6, $G$7, $G$8, $G$9, $G$10, $G$11, $G$312, $G$13, $G$14, $G$15,"]")</f>
         <v>[
   {
@@ -6455,584 +6526,584 @@
   }
 ]</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="44"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="37"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="37"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="37"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="44"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="37"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="44"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="37"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="44"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="37"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="44"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="37"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="37"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="44"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="37"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="44"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="37"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="44"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="37"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="44"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="37"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="44"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="37"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="44"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="37"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="44"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="37"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="44"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="37"/>
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="44"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="37"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="44"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="37"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="44"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="37"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="44"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="37"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="44"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="37"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="44"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="37"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="44"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="37"/>
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="44"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="37"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="44"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="37"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="44"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="37"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="44"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="37"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="44"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="37"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="44"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="37"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="44"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="37"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="44"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="37"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="44"/>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="37"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="44"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="37"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="44"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="37"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="44"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="37"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="44"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="37"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="44"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="37"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="44"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="37"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="44"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="37"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="37"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="44"/>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="37"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="44"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="37"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="44"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="37"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="44"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="37"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="44"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="37"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="44"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="37"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="37"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="44"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="37"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="44"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="37"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="44"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="37"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="44"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="37"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="37"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="44"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="37"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="44"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="44"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="37"/>
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="44"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="37"/>
+      <c r="A69" s="44"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="44"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="37"/>
+      <c r="A70" s="44"/>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="44"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="37"/>
+      <c r="A71" s="44"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="44"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="37"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="37"/>
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="44"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="37"/>
+      <c r="A73" s="44"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="44"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="37"/>
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="44"/>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="37"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="37"/>
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="44"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="37"/>
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="44"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="37"/>
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="44"/>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="37"/>
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="44"/>
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="37"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="37"/>
+      <c r="A79" s="44"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="44"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="37"/>
+      <c r="A80" s="44"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="44"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="37"/>
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="44"/>
     </row>
     <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="37"/>
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="44"/>
     </row>
     <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="37"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="37"/>
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="44"/>
     </row>
     <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="37"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="45"/>
+      <c r="E84" s="44"/>
     </row>
     <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="37"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="37"/>
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="45"/>
+      <c r="E85" s="44"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="37"/>
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="44"/>
     </row>
     <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="37"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="37"/>
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="44"/>
     </row>
     <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="37"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="37"/>
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="44"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="37"/>
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="45"/>
+      <c r="E89" s="44"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="37"/>
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="44"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="37"/>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="37"/>
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="45"/>
+      <c r="E91" s="44"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="37"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="37"/>
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="44"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="37"/>
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="37"/>
+      <c r="A93" s="44"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="45"/>
+      <c r="E93" s="44"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="37"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="37"/>
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="45"/>
+      <c r="E94" s="44"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="37"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="37"/>
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="45"/>
+      <c r="E95" s="44"/>
     </row>
     <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="37"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="37"/>
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="45"/>
+      <c r="E96" s="44"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="37"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="37"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="37"/>
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="45"/>
+      <c r="E97" s="44"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="37"/>
-      <c r="B98" s="37"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="37"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="45"/>
+      <c r="E98" s="44"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="37"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="37"/>
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="45"/>
+      <c r="E99" s="44"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7939,17 +8010,17 @@
     <mergeCell ref="A17:E99"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F15">
-    <cfRule type="beginsWith" dxfId="10" priority="2" operator="beginsWith" text="Valid">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="Valid">
       <formula>LEFT(F3,LEN("Valid"))="Valid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F15">
-    <cfRule type="beginsWith" dxfId="9" priority="4" operator="beginsWith" text="INVALID">
+    <cfRule type="beginsWith" dxfId="1" priority="4" operator="beginsWith" text="INVALID">
       <formula>LEFT(F3,LEN("INVALID"))="INVALID"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:E15">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>AND($B2="", $C2="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7985,6 +8056,150 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5737E0CB-5616-0C4F-9C56-87867202C2CC}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="25" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37"/>
+    </row>
+    <row r="4" spans="2:6" s="25" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="str">
+        <f>TRIM('Zendesk User Fields'!D3)</f>
+        <v>FNAME</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+    </row>
+    <row r="5" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B5" s="37"/>
+    </row>
+    <row r="6" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37"/>
+    </row>
+    <row r="8" spans="2:6" s="25" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="41" t="str">
+        <f>'Zendesk User Fields'!D4</f>
+        <v>LNAME</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B9" s="37"/>
+    </row>
+    <row r="10" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="36"/>
+    </row>
+    <row r="12" spans="2:6" s="25" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="41" t="str">
+        <f>'Zendesk User Fields'!D5</f>
+        <v>ZD_CUSTYPE</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B13" s="37"/>
+    </row>
+    <row r="14" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="36"/>
+    </row>
+    <row r="16" spans="2:6" s="25" customFormat="1" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="str">
+        <f>CLEAN('Zendesk User Fields'!A19)</f>
+        <v>[  {    "field_label" : "List of sites hosted (comma Seperated)",    "zendesk_field" : "site_list",    "mailchimp_field" : "SITES_LIST",    "type" : "text",    "default_value" : ""  },  {    "field_label" : "Mailchimp Footer Message",    "zendesk_field" : "mailchimp_footer_message",    "mailchimp_field" : "FOOTER_MSG",    "type" : "text",    "default_value" : ""  }]</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+    </row>
+    <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B17" s="37"/>
+    </row>
+    <row r="18" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="36"/>
+    </row>
+    <row r="20" spans="2:6" s="25" customFormat="1" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="42" t="str">
+        <f>CLEAN('Zendesk Organisation Fields'!A17)</f>
+        <v>[  {    "field_label" : "Our 'From' Email Address",    "zendesk_field" : "mailshot_success_email_address",    "mailchimp_field" : "FROMEMAIL",    "type" : "text",    "default_value" : "supportsteam@upnrunning.co.uk"  },  {    "field_label" : "Full URL of company Logo",    "zendesk_field" : "mailshot_company_logo_url",    "mailchimp_field" : "LOGO",    "type" : "image",    "default_value" : ""  },  {    "field_label" : "No of Employees",    "zendesk_field" : "no_of_employees",    "mailchimp_field" : "EMPLOYEES",    "type" : "text",    "default_value" : ""  },  {    "field_label" : "Year Customer Joined?",    "zendesk_field" : "year_customer_joined_us",    "mailchimp_field" : "STARTYEAR",    "type" : "text",    "default_value" : ""  }]</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+    </row>
+    <row r="21" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B21" s="37"/>
+    </row>
+    <row r="22" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="37"/>
+    </row>
+    <row r="24" spans="2:6" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="42" t="str">
+        <f>CLEAN('Mailchimp Only Fields'!A17)</f>
+        <v>[  {    "field_label" : "Maintenance Emails",    "mailchimp_field" : "SEND_MAINT",    "type" : "checkbox",    "value_if_ticked" : "Yes",    "value_if_unticked" : "No"  },  {    "field_label" : "VIP Promotion Emails",    "mailchimp_field" : "SEND_PROMO",    "type" : "checkbox",    "value_if_ticked" : "1",    "value_if_unticked" : "0"  },  {    "field_label" : "Monthly Scorecard Emails",    "mailchimp_field" : "SEND_SC",    "type" : "checkbox",    "value_if_ticked" : "0",    "value_if_unticked" : ""  }]</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Begun to build in proper comms between instances of app to keep info up to date when data is changed on 1 tab all other tabs will auto update to reflect change, ensuring you can trust the info that's shown in all tabs at all times
</commit_message>
<xml_diff>
--- a/extras/ZenchimpSettingsGenerator.xlsx
+++ b/extras/ZenchimpSettingsGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/ZenChimp-Zendesk-App-Mailchimp-Sync/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337758AE-265F-E340-921B-483A522F6983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE47233-EB1C-A341-B9D7-5038421B6F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Hidden" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
   <si>
     <t>Zendesk Field Types</t>
   </si>
@@ -341,6 +342,12 @@
   </si>
   <si>
     <t>Field Definitions for Mailchimp only fields*</t>
+  </si>
+  <si>
+    <t>Send</t>
+  </si>
+  <si>
+    <t>Don’t Send</t>
   </si>
 </sst>
 </file>
@@ -792,22 +799,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -825,6 +816,22 @@
     </xf>
     <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1234,14 +1241,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="27"/>
@@ -1297,13 +1304,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1350,9 +1357,9 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
@@ -2067,7 +2074,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="str">
+      <c r="A19" s="37" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$3, $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$314, $O$15, $O$16, $O$17,"]")</f>
         <v>[
   {
@@ -2086,651 +2093,651 @@
   }
 ]</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="43"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="43"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="43"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="43"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="43"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="43"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="43"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="43"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="43"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="43"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="43"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="43"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="43"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="43"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="43"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="43"/>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="43"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="43"/>
-      <c r="B62" s="43"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="43"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="43"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="43"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="43"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="43"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="43"/>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="43"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="43"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="43"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="43"/>
-      <c r="B72" s="43"/>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="43"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="43"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="43"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="43"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="43"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="43"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="43"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="43"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="43"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="43"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="43"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="43"/>
-      <c r="B81" s="43"/>
-      <c r="C81" s="43"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="43"/>
-      <c r="F81" s="43"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="43"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="43"/>
-      <c r="E82" s="43"/>
-      <c r="F82" s="43"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="43"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="43"/>
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="43"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="43"/>
-      <c r="B86" s="43"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="43"/>
-      <c r="B87" s="43"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="43"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="43"/>
-      <c r="B88" s="43"/>
-      <c r="C88" s="43"/>
-      <c r="D88" s="43"/>
-      <c r="E88" s="43"/>
-      <c r="F88" s="43"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="43"/>
-      <c r="B89" s="43"/>
-      <c r="C89" s="43"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="43"/>
-      <c r="F89" s="43"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="37"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="43"/>
-      <c r="B90" s="43"/>
-      <c r="C90" s="43"/>
-      <c r="D90" s="43"/>
-      <c r="E90" s="43"/>
-      <c r="F90" s="43"/>
+      <c r="A90" s="37"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="43"/>
-      <c r="B91" s="43"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-      <c r="F91" s="43"/>
+      <c r="A91" s="37"/>
+      <c r="B91" s="37"/>
+      <c r="C91" s="37"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="37"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="43"/>
-      <c r="B92" s="43"/>
-      <c r="C92" s="43"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="43"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="43"/>
-      <c r="B93" s="43"/>
-      <c r="C93" s="43"/>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="43"/>
-      <c r="B94" s="43"/>
-      <c r="C94" s="43"/>
-      <c r="D94" s="43"/>
-      <c r="E94" s="43"/>
-      <c r="F94" s="43"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="43"/>
-      <c r="B95" s="43"/>
-      <c r="C95" s="43"/>
-      <c r="D95" s="43"/>
-      <c r="E95" s="43"/>
-      <c r="F95" s="43"/>
+      <c r="A95" s="37"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="43"/>
-      <c r="B96" s="43"/>
-      <c r="C96" s="43"/>
-      <c r="D96" s="43"/>
-      <c r="E96" s="43"/>
-      <c r="F96" s="43"/>
+      <c r="A96" s="37"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="37"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="43"/>
-      <c r="B97" s="43"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="43"/>
-      <c r="E97" s="43"/>
-      <c r="F97" s="43"/>
+      <c r="A97" s="37"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="37"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="43"/>
-      <c r="B98" s="43"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="43"/>
-      <c r="E98" s="43"/>
-      <c r="F98" s="43"/>
+      <c r="A98" s="37"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="37"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="37"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="43"/>
-      <c r="B99" s="43"/>
-      <c r="C99" s="43"/>
-      <c r="D99" s="43"/>
-      <c r="E99" s="43"/>
-      <c r="F99" s="43"/>
+      <c r="A99" s="37"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="37"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3726,14 +3733,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -6148,8 +6155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0DBDDE-90C8-E44F-A66E-FB174AD2FD6F}">
   <dimension ref="A1:H998"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E99"/>
+    <sheetView topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6165,13 +6172,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
       <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6282,13 +6289,15 @@
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6"/>
+      <c r="D5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F5" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>Valid, but please make sure your values are valid for field type 'Text' and please make sure your Mailchimp field 'SEND_SC' is not marked as 'Required' as one of your values is blank</v>
+        <v>Valid, but please make sure your values are valid for field type 'Text'</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="2"/>
@@ -6296,8 +6305,8 @@
     "field_label" : "Monthly Scorecard Emails",
     "mailchimp_field" : "SEND_SC",
     "type" : "checkbox",
-    "value_if_ticked" : "0",
-    "value_if_unticked" : ""
+    "value_if_ticked" : "Send",
+    "value_if_unticked" : "Don’t Send"
   }
 </v>
       </c>
@@ -6521,8 +6530,8 @@
     "field_label" : "Monthly Scorecard Emails",
     "mailchimp_field" : "SEND_SC",
     "type" : "checkbox",
-    "value_if_ticked" : "0",
-    "value_if_unticked" : ""
+    "value_if_ticked" : "Send",
+    "value_if_unticked" : "Don’t Send"
   }
 ]</v>
       </c>
@@ -8059,8 +8068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5737E0CB-5616-0C4F-9C56-87867202C2CC}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8072,130 +8081,131 @@
   <sheetData>
     <row r="1" spans="2:6" s="25" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="32" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="2:6" s="25" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="str">
+      <c r="B4" s="35" t="str">
         <f>TRIM('Zendesk User Fields'!D3)</f>
         <v>FNAME</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="37"/>
+      <c r="B5" s="31"/>
     </row>
     <row r="6" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="32" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="7" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
+      <c r="B7" s="31"/>
     </row>
     <row r="8" spans="2:6" s="25" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="str">
+      <c r="B8" s="35" t="str">
         <f>'Zendesk User Fields'!D4</f>
         <v>LNAME</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
+      <c r="B9" s="31"/>
     </row>
     <row r="10" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="32" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
+      <c r="B11" s="30"/>
     </row>
     <row r="12" spans="2:6" s="25" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="str">
+      <c r="B12" s="35" t="str">
         <f>'Zendesk User Fields'!D5</f>
         <v>ZD_CUSTYPE</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="37"/>
+      <c r="B13" s="31"/>
     </row>
     <row r="14" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="32" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
+      <c r="B15" s="30"/>
     </row>
     <row r="16" spans="2:6" s="25" customFormat="1" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="str">
+      <c r="B16" s="36" t="str">
         <f>CLEAN('Zendesk User Fields'!A19)</f>
         <v>[  {    "field_label" : "List of sites hosted (comma Seperated)",    "zendesk_field" : "site_list",    "mailchimp_field" : "SITES_LIST",    "type" : "text",    "default_value" : ""  },  {    "field_label" : "Mailchimp Footer Message",    "zendesk_field" : "mailchimp_footer_message",    "mailchimp_field" : "FOOTER_MSG",    "type" : "text",    "default_value" : ""  }]</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="37"/>
+      <c r="B17" s="31"/>
     </row>
     <row r="18" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="32" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="25" customFormat="1" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
+      <c r="B19" s="30"/>
     </row>
     <row r="20" spans="2:6" s="25" customFormat="1" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="42" t="str">
+      <c r="B20" s="36" t="str">
         <f>CLEAN('Zendesk Organisation Fields'!A17)</f>
         <v>[  {    "field_label" : "Our 'From' Email Address",    "zendesk_field" : "mailshot_success_email_address",    "mailchimp_field" : "FROMEMAIL",    "type" : "text",    "default_value" : "supportsteam@upnrunning.co.uk"  },  {    "field_label" : "Full URL of company Logo",    "zendesk_field" : "mailshot_company_logo_url",    "mailchimp_field" : "LOGO",    "type" : "image",    "default_value" : ""  },  {    "field_label" : "No of Employees",    "zendesk_field" : "no_of_employees",    "mailchimp_field" : "EMPLOYEES",    "type" : "text",    "default_value" : ""  },  {    "field_label" : "Year Customer Joined?",    "zendesk_field" : "year_customer_joined_us",    "mailchimp_field" : "STARTYEAR",    "type" : "text",    "default_value" : ""  }]</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B21" s="37"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="2:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="32" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="2:6" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="str">
+      <c r="B24" s="36" t="str">
         <f>CLEAN('Mailchimp Only Fields'!A17)</f>
-        <v>[  {    "field_label" : "Maintenance Emails",    "mailchimp_field" : "SEND_MAINT",    "type" : "checkbox",    "value_if_ticked" : "Yes",    "value_if_unticked" : "No"  },  {    "field_label" : "VIP Promotion Emails",    "mailchimp_field" : "SEND_PROMO",    "type" : "checkbox",    "value_if_ticked" : "1",    "value_if_unticked" : "0"  },  {    "field_label" : "Monthly Scorecard Emails",    "mailchimp_field" : "SEND_SC",    "type" : "checkbox",    "value_if_ticked" : "0",    "value_if_unticked" : ""  }]</v>
-      </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+        <v>[  {    "field_label" : "Maintenance Emails",    "mailchimp_field" : "SEND_MAINT",    "type" : "checkbox",    "value_if_ticked" : "Yes",    "value_if_unticked" : "No"  },  {    "field_label" : "VIP Promotion Emails",    "mailchimp_field" : "SEND_PROMO",    "type" : "checkbox",    "value_if_ticked" : "1",    "value_if_unticked" : "0"  },  {    "field_label" : "Monthly Scorecard Emails",    "mailchimp_field" : "SEND_SC",    "type" : "checkbox",    "value_if_ticked" : "Send",    "value_if_unticked" : "Don’t Send"  }]</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>